<commit_message>
Updates to spreadsheet from Ken.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\prototype-historical-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D3C94D-619A-4A14-94C7-D0A5E2FA8597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4679ED-61A9-41DB-931E-F8C724273F2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="141">
   <si>
     <t>start_year</t>
   </si>
@@ -443,15 +443,6 @@
   </si>
   <si>
     <t>layer_name</t>
-  </si>
-  <si>
-    <t>Am I correct: was this a highway project?</t>
-  </si>
-  <si>
-    <t>Is the type 't' or 'z'? Does this layer have an end_date?</t>
-  </si>
-  <si>
-    <t>What is the start_date for this layer?</t>
   </si>
 </sst>
 </file>
@@ -776,7 +767,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1302,7 +1293,7 @@
   <dimension ref="A1:E131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E112" sqref="E112"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,6 +1469,9 @@
       <c r="B12">
         <v>1807</v>
       </c>
+      <c r="C12">
+        <v>9999</v>
+      </c>
       <c r="D12" t="s">
         <v>137</v>
       </c>
@@ -1487,7 +1481,10 @@
         <v>14</v>
       </c>
       <c r="B13">
-        <v>1908</v>
+        <v>1809</v>
+      </c>
+      <c r="C13">
+        <v>9999</v>
       </c>
       <c r="D13" t="s">
         <v>137</v>
@@ -1500,6 +1497,9 @@
       <c r="B14">
         <v>1868</v>
       </c>
+      <c r="C14">
+        <v>9999</v>
+      </c>
       <c r="D14" t="s">
         <v>137</v>
       </c>
@@ -1525,6 +1525,9 @@
       <c r="B16">
         <v>1838</v>
       </c>
+      <c r="C16">
+        <v>9999</v>
+      </c>
       <c r="D16" t="s">
         <v>137</v>
       </c>
@@ -1536,6 +1539,9 @@
       <c r="B17">
         <v>1829</v>
       </c>
+      <c r="C17">
+        <v>9999</v>
+      </c>
       <c r="D17" t="s">
         <v>137</v>
       </c>
@@ -1547,6 +1553,9 @@
       <c r="B18">
         <v>1830</v>
       </c>
+      <c r="C18">
+        <v>9999</v>
+      </c>
       <c r="D18" t="s">
         <v>137</v>
       </c>
@@ -1572,6 +1581,9 @@
       <c r="B20">
         <v>1857</v>
       </c>
+      <c r="C20">
+        <v>9999</v>
+      </c>
       <c r="D20" t="s">
         <v>137</v>
       </c>
@@ -1597,6 +1609,9 @@
       <c r="B22">
         <v>1845</v>
       </c>
+      <c r="C22">
+        <v>9999</v>
+      </c>
       <c r="D22" t="s">
         <v>137</v>
       </c>
@@ -1608,6 +1623,9 @@
       <c r="B23">
         <v>1805</v>
       </c>
+      <c r="C23">
+        <v>9999</v>
+      </c>
       <c r="D23" t="s">
         <v>137</v>
       </c>
@@ -1738,7 +1756,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1752,7 +1770,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1766,7 +1784,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1780,7 +1798,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1794,7 +1812,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1808,7 +1826,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1822,7 +1840,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1832,22 +1850,25 @@
       <c r="C39">
         <v>9999</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="D39" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40">
         <v>1875</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>9999</v>
+      </c>
+      <c r="D40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1861,7 +1882,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1875,7 +1896,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1889,7 +1910,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1903,7 +1924,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1917,7 +1938,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1931,7 +1952,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1945,7 +1966,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -2232,6 +2253,9 @@
       <c r="A68" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="B68" s="1">
+        <v>1964</v>
+      </c>
       <c r="C68" s="1">
         <v>9999</v>
       </c>
@@ -2239,7 +2263,7 @@
         <v>137</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>143</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2634,7 +2658,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -2648,7 +2672,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>100</v>
       </c>
@@ -2662,7 +2686,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>101</v>
       </c>
@@ -2676,7 +2700,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>102</v>
       </c>
@@ -2690,7 +2714,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>103</v>
       </c>
@@ -2704,7 +2728,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>104</v>
       </c>
@@ -2718,7 +2742,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>105</v>
       </c>
@@ -2732,7 +2756,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>106</v>
       </c>
@@ -2746,7 +2770,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -2760,7 +2784,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>108</v>
       </c>
@@ -2774,7 +2798,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>109</v>
       </c>
@@ -2788,7 +2812,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>110</v>
       </c>
@@ -2802,7 +2826,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>111</v>
       </c>
@@ -2816,7 +2840,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>112</v>
       </c>
@@ -2830,7 +2854,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>113</v>
       </c>
@@ -2844,7 +2868,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="112" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>114</v>
       </c>
@@ -2856,9 +2880,6 @@
       </c>
       <c r="D112" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Reflects updates from Ken 12/13/2020 @ 9:55 a.m.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\prototype-historical-map\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA42248-876F-407C-A60B-3B8734A6EF5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF8C17E-9E7D-4E67-95C7-BF6EDA0E21F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="210" windowWidth="19995" windowHeight="11580" xr2:uid="{48B35B47-D791-4DB0-8E3F-11AF1DC17D23}"/>
+    <workbookView xWindow="510" yWindow="1425" windowWidth="19995" windowHeight="10155" xr2:uid="{48B35B47-D791-4DB0-8E3F-11AF1DC17D23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="362">
   <si>
     <t>Salem Turnpike (Rt. 107)</t>
   </si>
@@ -393,12 +393,6 @@
     <t>Massport takes control of  Hanscom Field</t>
   </si>
   <si>
-    <t>Orange Line (Malden–Oak Grove)</t>
-  </si>
-  <si>
-    <t>Newburyport CR line (beyond Ipswich, closed) 1976</t>
-  </si>
-  <si>
     <t>Fairmount CR line</t>
   </si>
   <si>
@@ -1114,6 +1108,9 @@
   </si>
   <si>
     <t>layer_name</t>
+  </si>
+  <si>
+    <t>Orange Line (Sullivan–Oak Grove)</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1172,9 +1169,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1493,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB246BE0-9101-4910-B137-94A0FD6048BC}">
-  <dimension ref="A1:E201"/>
+  <dimension ref="A1:E200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,24 +1504,24 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -1536,12 +1530,12 @@
         <v>9999</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -1550,12 +1544,12 @@
         <v>9999</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -1564,12 +1558,12 @@
         <v>9999</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -1578,12 +1572,12 @@
         <v>9999</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -1592,12 +1586,12 @@
         <v>9999</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -1606,12 +1600,12 @@
         <v>9999</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -1620,12 +1614,12 @@
         <v>9999</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -1634,12 +1628,12 @@
         <v>9999</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -1648,12 +1642,12 @@
         <v>9999</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
@@ -1662,12 +1656,12 @@
         <v>9999</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>0</v>
@@ -1679,12 +1673,12 @@
         <v>1868</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
@@ -1696,12 +1690,12 @@
         <v>1838</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
@@ -1713,12 +1707,12 @@
         <v>9999</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -1730,12 +1724,12 @@
         <v>1857</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
@@ -1747,12 +1741,12 @@
         <v>1829</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>5</v>
@@ -1764,12 +1758,12 @@
         <v>1845</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -1781,12 +1775,12 @@
         <v>1830</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
@@ -1798,12 +1792,12 @@
         <v>1841</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>8</v>
@@ -1815,12 +1809,12 @@
         <v>9999</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>9</v>
@@ -1832,12 +1826,12 @@
         <v>9999</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>11</v>
@@ -1849,12 +1843,12 @@
         <v>1849</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>10</v>
@@ -1866,15 +1860,15 @@
         <v>1871</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C24" s="4">
         <v>1829</v>
@@ -1883,15 +1877,15 @@
         <v>9999</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B25" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C25" s="4">
         <v>1830</v>
@@ -1900,12 +1894,12 @@
         <v>9999</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>12</v>
@@ -1917,12 +1911,12 @@
         <v>9999</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
@@ -1934,12 +1928,12 @@
         <v>9999</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>14</v>
@@ -1951,15 +1945,15 @@
         <v>9999</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C29" s="4">
         <v>1838</v>
@@ -1968,12 +1962,12 @@
         <v>9999</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>15</v>
@@ -1985,12 +1979,12 @@
         <v>9999</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>16</v>
@@ -1998,16 +1992,16 @@
       <c r="C31" s="2">
         <v>1839</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="4">
         <v>1976</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>17</v>
@@ -2019,12 +2013,12 @@
         <v>9999</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>18</v>
@@ -2036,12 +2030,12 @@
         <v>1961</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>19</v>
@@ -2053,12 +2047,12 @@
         <v>9999</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>20</v>
@@ -2070,15 +2064,15 @@
         <v>1966</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C36" s="4">
         <v>1845</v>
@@ -2087,12 +2081,12 @@
         <v>9999</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>21</v>
@@ -2104,12 +2098,12 @@
         <v>9999</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>22</v>
@@ -2121,12 +2115,12 @@
         <v>1959</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>23</v>
@@ -2138,12 +2132,12 @@
         <v>1959</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>27</v>
@@ -2155,12 +2149,12 @@
         <v>1936</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>26</v>
@@ -2172,12 +2166,12 @@
         <v>1941</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>25</v>
@@ -2189,12 +2183,12 @@
         <v>1943</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>24</v>
@@ -2206,12 +2200,12 @@
         <v>1981</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>34</v>
@@ -2223,12 +2217,12 @@
         <v>9999</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>33</v>
@@ -2240,12 +2234,12 @@
         <v>1863</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>32</v>
@@ -2257,12 +2251,12 @@
         <v>1960</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>31</v>
@@ -2274,12 +2268,12 @@
         <v>1960</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>30</v>
@@ -2291,12 +2285,12 @@
         <v>1980</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>29</v>
@@ -2308,12 +2302,12 @@
         <v>1980</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>28</v>
@@ -2325,12 +2319,12 @@
         <v>1985</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>35</v>
@@ -2342,12 +2336,12 @@
         <v>1861</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>36</v>
@@ -2359,12 +2353,12 @@
         <v>1972</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>37</v>
@@ -2376,12 +2370,12 @@
         <v>1981</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>38</v>
@@ -2393,12 +2387,12 @@
         <v>2011</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>40</v>
@@ -2410,12 +2404,12 @@
         <v>9999</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>39</v>
@@ -2427,12 +2421,12 @@
         <v>1992</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>41</v>
@@ -2444,12 +2438,12 @@
         <v>9999</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>42</v>
@@ -2461,12 +2455,12 @@
         <v>1980</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>43</v>
@@ -2478,12 +2472,12 @@
         <v>9999</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>44</v>
@@ -2495,12 +2489,12 @@
         <v>1993</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>45</v>
@@ -2512,12 +2506,12 @@
         <v>1987</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>47</v>
@@ -2529,12 +2523,12 @@
         <v>1927</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>46</v>
@@ -2546,12 +2540,12 @@
         <v>1958</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>48</v>
@@ -2563,12 +2557,12 @@
         <v>1981</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="8" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>49</v>
@@ -2580,15 +2574,15 @@
         <v>1912</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C66" s="4">
         <v>1857</v>
@@ -2597,12 +2591,12 @@
         <v>9999</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>50</v>
@@ -2614,12 +2608,12 @@
         <v>9999</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>51</v>
@@ -2631,12 +2625,12 @@
         <v>1976</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>52</v>
@@ -2648,15 +2642,15 @@
         <v>1993</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C70" s="4">
         <v>1868</v>
@@ -2665,12 +2659,12 @@
         <v>9999</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>53</v>
@@ -2682,12 +2676,12 @@
         <v>2001</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>54</v>
@@ -2699,12 +2693,12 @@
         <v>1993</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>55</v>
@@ -2716,12 +2710,12 @@
         <v>1924</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>56</v>
@@ -2733,12 +2727,12 @@
         <v>1920</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>57</v>
@@ -2750,12 +2744,12 @@
         <v>1979</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>58</v>
@@ -2767,12 +2761,12 @@
         <v>1961</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="8" t="s">
-        <v>320</v>
+      <c r="A77" s="7" t="s">
+        <v>318</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>59</v>
@@ -2784,12 +2778,12 @@
         <v>9999</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>60</v>
@@ -2801,12 +2795,12 @@
         <v>1919</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>61</v>
@@ -2818,12 +2812,12 @@
         <v>9999</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>62</v>
@@ -2835,12 +2829,12 @@
         <v>9999</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>63</v>
@@ -2852,12 +2846,12 @@
         <v>9999</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>64</v>
@@ -2869,12 +2863,12 @@
         <v>9999</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>66</v>
@@ -2886,12 +2880,12 @@
         <v>1987</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>65</v>
@@ -2903,12 +2897,12 @@
         <v>1938</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>67</v>
@@ -2920,12 +2914,12 @@
         <v>9999</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>68</v>
@@ -2937,12 +2931,12 @@
         <v>9999</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>69</v>
@@ -2954,12 +2948,12 @@
         <v>9999</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>70</v>
@@ -2971,12 +2965,12 @@
         <v>9999</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>71</v>
@@ -2988,12 +2982,12 @@
         <v>1987</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>72</v>
@@ -3005,12 +2999,12 @@
         <v>9999</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>73</v>
@@ -3022,12 +3016,12 @@
         <v>9999</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>74</v>
@@ -3039,12 +3033,12 @@
         <v>9999</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>75</v>
@@ -3056,12 +3050,12 @@
         <v>9999</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>76</v>
@@ -3073,12 +3067,12 @@
         <v>9999</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>77</v>
@@ -3090,12 +3084,12 @@
         <v>9999</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>78</v>
@@ -3107,12 +3101,12 @@
         <v>9999</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>79</v>
@@ -3124,12 +3118,12 @@
         <v>2009</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>80</v>
@@ -3141,12 +3135,12 @@
         <v>1975</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>81</v>
@@ -3158,12 +3152,12 @@
         <v>9999</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>83</v>
@@ -3175,12 +3169,12 @@
         <v>9999</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>82</v>
@@ -3192,12 +3186,12 @@
         <v>9999</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>84</v>
@@ -3209,12 +3203,12 @@
         <v>9999</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>85</v>
@@ -3226,12 +3220,12 @@
         <v>9999</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>87</v>
@@ -3243,12 +3237,12 @@
         <v>9999</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>86</v>
@@ -3260,12 +3254,12 @@
         <v>1963</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>89</v>
@@ -3277,12 +3271,12 @@
         <v>9999</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>88</v>
@@ -3294,12 +3288,12 @@
         <v>9999</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>90</v>
@@ -3311,12 +3305,12 @@
         <v>9999</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>91</v>
@@ -3328,12 +3322,12 @@
         <v>1964</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>92</v>
@@ -3345,12 +3339,12 @@
         <v>9999</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>93</v>
@@ -3362,15 +3356,15 @@
         <v>9999</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C112" s="2">
         <v>1952</v>
@@ -3379,12 +3373,12 @@
         <v>9999</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>95</v>
@@ -3396,12 +3390,12 @@
         <v>2009</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>94</v>
@@ -3413,12 +3407,12 @@
         <v>9999</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>97</v>
@@ -3430,12 +3424,12 @@
         <v>9999</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>98</v>
@@ -3447,12 +3441,12 @@
         <v>9999</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>96</v>
@@ -3464,12 +3458,12 @@
         <v>9999</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>99</v>
@@ -3481,12 +3475,12 @@
         <v>9999</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>100</v>
@@ -3498,15 +3492,15 @@
         <v>9999</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C120" s="2">
         <v>1957</v>
@@ -3515,12 +3509,12 @@
         <v>2016</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>102</v>
@@ -3532,12 +3526,12 @@
         <v>9999</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>101</v>
@@ -3549,12 +3543,12 @@
         <v>9999</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>103</v>
@@ -3566,12 +3560,12 @@
         <v>9999</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>104</v>
@@ -3583,12 +3577,12 @@
         <v>9999</v>
       </c>
       <c r="E124" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>105</v>
@@ -3600,15 +3594,15 @@
         <v>9999</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C126" s="2">
         <v>1959</v>
@@ -3617,15 +3611,15 @@
         <v>2004</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C127" s="2">
         <v>1959</v>
@@ -3634,12 +3628,12 @@
         <v>9999</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>106</v>
@@ -3651,12 +3645,12 @@
         <v>9999</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B129" s="5" t="s">
         <v>107</v>
@@ -3668,12 +3662,12 @@
         <v>9999</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>108</v>
@@ -3685,15 +3679,15 @@
         <v>9999</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C131" s="2">
         <v>1962</v>
@@ -3702,12 +3696,12 @@
         <v>9999</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>109</v>
@@ -3719,12 +3713,12 @@
         <v>9999</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>110</v>
@@ -3736,12 +3730,12 @@
         <v>9999</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>112</v>
@@ -3753,12 +3747,12 @@
         <v>9999</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>113</v>
@@ -3770,12 +3764,12 @@
         <v>9999</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>111</v>
@@ -3787,12 +3781,12 @@
         <v>9999</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>114</v>
@@ -3804,7 +3798,7 @@
         <v>9999</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3818,12 +3812,12 @@
         <v>9999</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>115</v>
@@ -3835,12 +3829,12 @@
         <v>9999</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>117</v>
@@ -3852,12 +3846,12 @@
         <v>9999</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>118</v>
@@ -3869,15 +3863,15 @@
         <v>9999</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="8" t="s">
-        <v>318</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="7" t="s">
+        <v>316</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C142" s="4">
         <v>1970</v>
@@ -3886,12 +3880,12 @@
         <v>9999</v>
       </c>
       <c r="E142" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>119</v>
@@ -3903,12 +3897,12 @@
         <v>9999</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>120</v>
@@ -3920,12 +3914,12 @@
         <v>9999</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>121</v>
@@ -3937,15 +3931,15 @@
         <v>9999</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C146" s="2">
         <v>1975</v>
@@ -3954,15 +3948,15 @@
         <v>9999</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C147" s="4">
         <v>1975</v>
@@ -3971,15 +3965,15 @@
         <v>9999</v>
       </c>
       <c r="E147" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C148" s="4">
         <v>1975</v>
@@ -3988,115 +3982,117 @@
         <v>9999</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="149" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="6"/>
-      <c r="B149" s="6" t="s">
+      <c r="A149" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C149" s="4">
+        <v>1975</v>
+      </c>
+      <c r="D149" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C150" s="2">
+        <v>1979</v>
+      </c>
+      <c r="D150" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C151" s="4">
+        <v>1980</v>
+      </c>
+      <c r="D151" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B152" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C149" s="3">
-        <v>1976</v>
-      </c>
-      <c r="D149" s="3">
-        <v>1976</v>
-      </c>
-      <c r="E149" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="B150" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C150" s="4">
-        <v>1975</v>
-      </c>
-      <c r="D150" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E150" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C151" s="2">
-        <v>1979</v>
-      </c>
-      <c r="D151" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="B152" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C152" s="4">
-        <v>1980</v>
-      </c>
-      <c r="D152" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E152" s="4" t="s">
-        <v>181</v>
+      <c r="C152" s="2">
+        <v>1984</v>
+      </c>
+      <c r="D152" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C153" s="2">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="D153" s="2">
         <v>9999</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="C154" s="2">
-        <v>1985</v>
+        <v>1987</v>
       </c>
       <c r="D154" s="2">
         <v>9999</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C155" s="2">
         <v>1987</v>
@@ -4105,32 +4101,32 @@
         <v>9999</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="C156" s="2">
-        <v>1987</v>
+        <v>1992</v>
       </c>
       <c r="D156" s="2">
         <v>9999</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C157" s="2">
         <v>1992</v>
@@ -4139,100 +4135,100 @@
         <v>9999</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C158" s="2">
-        <v>1992</v>
-      </c>
-      <c r="D158" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E158" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C158" s="4">
+        <v>1993</v>
+      </c>
+      <c r="D158" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B159" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C159" s="4">
+        <v>1994</v>
+      </c>
+      <c r="D159" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>301</v>
+      </c>
+      <c r="B160" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C159" s="4">
-        <v>1993</v>
-      </c>
-      <c r="D159" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E159" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B160" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C160" s="4">
+      <c r="C160" s="2">
         <v>1994</v>
       </c>
-      <c r="D160" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E160" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>303</v>
-      </c>
-      <c r="B161" s="1" t="s">
+      <c r="D160" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B161" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C161" s="2">
-        <v>1994</v>
-      </c>
-      <c r="D161" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E161" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C161" s="4">
+        <v>1995</v>
+      </c>
+      <c r="D161" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C162" s="4">
+        <v>280</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C162" s="2">
         <v>1995</v>
       </c>
-      <c r="D162" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E162" s="4" t="s">
-        <v>179</v>
+      <c r="D162" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>282</v>
+        <v>235</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C163" s="2">
         <v>1995</v>
@@ -4246,197 +4242,197 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>237</v>
+        <v>279</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C164" s="2">
-        <v>1995</v>
+        <v>1997</v>
       </c>
       <c r="D164" s="2">
         <v>9999</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="B165" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B165" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C165" s="2">
-        <v>1997</v>
-      </c>
-      <c r="D165" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E165" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B166" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C166" s="4">
+      <c r="C165" s="4">
         <v>1998</v>
       </c>
-      <c r="D166" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E166" s="4" t="s">
-        <v>185</v>
+      <c r="D165" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E165" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>278</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C166" s="2">
+        <v>1998</v>
+      </c>
+      <c r="D166" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C167" s="2">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="D167" s="2">
         <v>9999</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B168" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C168" s="2">
+        <v>2002</v>
+      </c>
+      <c r="D168" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B169" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C168" s="2">
-        <v>1999</v>
-      </c>
-      <c r="D168" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E168" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>279</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C169" s="2">
+      <c r="C169" s="4">
         <v>2002</v>
       </c>
-      <c r="D169" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E169" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B170" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C170" s="4">
+      <c r="D169" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E169" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>275</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C170" s="2">
         <v>2002</v>
       </c>
-      <c r="D170" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E170" s="4" t="s">
+      <c r="D170" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E170" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C171" s="2">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="D171" s="2">
         <v>9999</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>276</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C172" s="2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C172" s="4">
         <v>2003</v>
       </c>
-      <c r="D172" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E172" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B173" s="5" t="s">
+      <c r="D172" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E172" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>273</v>
+      </c>
+      <c r="B173" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C173" s="4">
+      <c r="C173" s="2">
         <v>2003</v>
       </c>
-      <c r="D173" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E173" s="4" t="s">
+      <c r="D173" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E173" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B174" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C174" s="2">
+        <v>2005</v>
+      </c>
+      <c r="D174" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B175" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="C174" s="2">
-        <v>2003</v>
-      </c>
-      <c r="D174" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E174" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>274</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>357</v>
       </c>
       <c r="C175" s="2">
         <v>2005</v>
@@ -4445,15 +4441,15 @@
         <v>9999</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C176" s="2">
         <v>2005</v>
@@ -4462,49 +4458,49 @@
         <v>9999</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="5" t="s">
-        <v>237</v>
+      <c r="A177" t="s">
+        <v>271</v>
       </c>
       <c r="B177" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C177" s="2">
+        <v>2006</v>
+      </c>
+      <c r="D177" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B178" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C177" s="2">
-        <v>2005</v>
-      </c>
-      <c r="D177" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E177" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>273</v>
-      </c>
-      <c r="B178" s="1" t="s">
-        <v>356</v>
-      </c>
       <c r="C178" s="2">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="D178" s="2">
         <v>9999</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>272</v>
+        <v>352</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>151</v>
+        <v>353</v>
       </c>
       <c r="C179" s="2">
         <v>2007</v>
@@ -4513,66 +4509,66 @@
         <v>9999</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="5" t="s">
-        <v>354</v>
+      <c r="A180" t="s">
+        <v>264</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>355</v>
+        <v>151</v>
       </c>
       <c r="C180" s="2">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="D180" s="2">
         <v>9999</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>266</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C181" s="2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C181" s="4">
         <v>2008</v>
       </c>
-      <c r="D181" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E181" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="182" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B182" s="5" t="s">
+      <c r="D181" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E181" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>261</v>
+      </c>
+      <c r="B182" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C182" s="4">
-        <v>2008</v>
-      </c>
-      <c r="D182" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E182" s="4" t="s">
-        <v>185</v>
+      <c r="C182" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D182" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>263</v>
+      <c r="A183" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="C183" s="2">
         <v>2009</v>
@@ -4581,15 +4577,15 @@
         <v>9999</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" s="5" t="s">
-        <v>237</v>
+      <c r="A184" t="s">
+        <v>262</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="C184" s="2">
         <v>2009</v>
@@ -4598,49 +4594,49 @@
         <v>9999</v>
       </c>
       <c r="E184" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C185" s="4">
+        <v>2010</v>
+      </c>
+      <c r="D185" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E185" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>264</v>
-      </c>
-      <c r="B185" s="1" t="s">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>263</v>
+      </c>
+      <c r="B186" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C185" s="2">
-        <v>2009</v>
-      </c>
-      <c r="D185" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E185" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B186" s="5" t="s">
+      <c r="C186" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D186" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B187" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="C186" s="4">
-        <v>2010</v>
-      </c>
-      <c r="D186" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E186" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>265</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="C187" s="2">
         <v>2012</v>
@@ -4649,80 +4645,80 @@
         <v>9999</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="5" t="s">
-        <v>271</v>
+      <c r="A188" t="s">
+        <v>260</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C188" s="2">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D188" s="2">
         <v>9999</v>
       </c>
       <c r="E188" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B189" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C189" s="2">
+        <v>2014</v>
+      </c>
+      <c r="D189" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B190" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C189" s="2">
-        <v>2013</v>
-      </c>
-      <c r="D189" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E189" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
+      <c r="C190" s="4">
+        <v>2014</v>
+      </c>
+      <c r="D190" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E190" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C191" s="2">
+        <v>2015</v>
+      </c>
+      <c r="D191" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>267</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C190" s="2">
-        <v>2014</v>
-      </c>
-      <c r="D190" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E190" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B191" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C191" s="4">
-        <v>2014</v>
-      </c>
-      <c r="D191" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E191" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="5" t="s">
-        <v>268</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>162</v>
@@ -4734,15 +4730,15 @@
         <v>9999</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C193" s="2">
         <v>2015</v>
@@ -4751,83 +4747,83 @@
         <v>9999</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>270</v>
-      </c>
-      <c r="B194" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B194" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C194" s="2">
-        <v>2015</v>
-      </c>
-      <c r="D194" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E194" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C194" s="4">
+        <v>2016</v>
+      </c>
+      <c r="D194" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E194" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B195" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C195" s="4">
+        <v>2017</v>
+      </c>
+      <c r="D195" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E195" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C196" s="4">
+        <v>2018</v>
+      </c>
+      <c r="D196" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E196" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C197" s="2">
+        <v>2018</v>
+      </c>
+      <c r="D197" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E197" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>259</v>
+      </c>
+      <c r="B198" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="C195" s="4">
-        <v>2016</v>
-      </c>
-      <c r="D195" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E195" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B196" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C196" s="4">
-        <v>2017</v>
-      </c>
-      <c r="D196" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E196" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="8" t="s">
-        <v>305</v>
-      </c>
-      <c r="B197" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="C197" s="4">
-        <v>2018</v>
-      </c>
-      <c r="D197" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E197" s="4" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="C198" s="2">
         <v>2018</v>
@@ -4836,64 +4832,47 @@
         <v>9999</v>
       </c>
       <c r="E198" s="2" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>167</v>
       </c>
       <c r="C199" s="2">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="D199" s="2">
         <v>9999</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C200" s="2">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="D200" s="2">
         <v>9999</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>258</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C201" s="2">
-        <v>2021</v>
-      </c>
-      <c r="D201" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E201" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E201">
-    <sortCondition ref="C2:C201"/>
-    <sortCondition ref="E2:E201"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E200">
+    <sortCondition ref="C2:C200"/>
+    <sortCondition ref="E2:E200"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Addition of rows for Providence CR, Stoughton CR, fix to Salem-Turnpike and Route-3-Norwell-Boston.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\prototype-historical-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF8C17E-9E7D-4E67-95C7-BF6EDA0E21F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B43E6ED-CFF5-4FC1-8BC8-F5B3B69BA710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="510" yWindow="1425" windowWidth="19995" windowHeight="10155" xr2:uid="{48B35B47-D791-4DB0-8E3F-11AF1DC17D23}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{48B35B47-D791-4DB0-8E3F-11AF1DC17D23}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="367">
   <si>
     <t>Salem Turnpike (Rt. 107)</t>
   </si>
@@ -741,15 +741,6 @@
     <t>Logan-Airport-1923</t>
   </si>
   <si>
-    <t>Red_LIne-1927</t>
-  </si>
-  <si>
-    <t>Red_LIne-1928</t>
-  </si>
-  <si>
-    <t>Red_LIne-1929</t>
-  </si>
-  <si>
     <t>Sumner-Tunnel-1934</t>
   </si>
   <si>
@@ -1080,9 +1071,6 @@
     <t>I-93_SE_Expressway_Rt.3_Rt.24_I-95</t>
   </si>
   <si>
-    <t>Route-3-Boston-Norwell-1957</t>
-  </si>
-  <si>
     <t>Greenbush-CR-2007</t>
   </si>
   <si>
@@ -1111,6 +1099,33 @@
   </si>
   <si>
     <t>Orange Line (Sullivan–Oak Grove)</t>
+  </si>
+  <si>
+    <t>Route-3-Norwell-Boston-1957</t>
+  </si>
+  <si>
+    <t>Salem-Turnpike-1803-1868</t>
+  </si>
+  <si>
+    <t>Providence-CR-1834</t>
+  </si>
+  <si>
+    <t>Providence CR Line (Providence-Boston)</t>
+  </si>
+  <si>
+    <t>Stoughton-CR-1888</t>
+  </si>
+  <si>
+    <t>Stoughton CR Line</t>
+  </si>
+  <si>
+    <t>Red_Line-1929</t>
+  </si>
+  <si>
+    <t>Red_Line-1927</t>
+  </si>
+  <si>
+    <t>Red_Line-1928</t>
   </si>
 </sst>
 </file>
@@ -1487,10 +1502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB246BE0-9101-4910-B137-94A0FD6048BC}">
-  <dimension ref="A1:E200"/>
+  <dimension ref="A1:E202"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,7 +1519,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>175</v>
@@ -1661,7 +1676,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>359</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>0</v>
@@ -1865,10 +1880,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C24" s="4">
         <v>1829</v>
@@ -1882,10 +1897,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B25" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C25" s="4">
         <v>1830</v>
@@ -1914,86 +1929,86 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1834</v>
+      </c>
+      <c r="D27" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C28" s="2">
         <v>1835</v>
       </c>
-      <c r="D27" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="D28" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C29" s="2">
         <v>1837</v>
       </c>
-      <c r="D28" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>306</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="C29" s="4">
+      <c r="D29" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>303</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="C30" s="4">
         <v>1838</v>
       </c>
-      <c r="D29" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="2">
-        <v>1838</v>
-      </c>
-      <c r="D30" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>180</v>
+      <c r="D30" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="2">
-        <v>1839</v>
-      </c>
-      <c r="D31" s="4">
-        <v>1976</v>
+        <v>1838</v>
+      </c>
+      <c r="D31" s="2">
+        <v>9999</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>180</v>
@@ -2001,16 +2016,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32" s="2">
-        <v>1843</v>
-      </c>
-      <c r="D32" s="2">
-        <v>9999</v>
+        <v>1839</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1976</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>180</v>
@@ -2018,152 +2033,152 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1843</v>
+      </c>
+      <c r="D33" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C33" s="2">
-        <v>1844</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1961</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>209</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="C34" s="2">
         <v>1844</v>
       </c>
       <c r="D34" s="2">
-        <v>9999</v>
+        <v>1961</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>210</v>
+      <c r="A35" t="s">
+        <v>209</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35" s="2">
         <v>1844</v>
       </c>
       <c r="D35" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1844</v>
+      </c>
+      <c r="D36" s="2">
         <v>1966</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>307</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="C36" s="4">
+      <c r="E36" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>304</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="C37" s="4">
         <v>1845</v>
       </c>
-      <c r="D36" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="D37" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C37" s="2">
-        <v>1845</v>
-      </c>
-      <c r="D37" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="C38" s="2">
         <v>1845</v>
       </c>
       <c r="D38" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1845</v>
+      </c>
+      <c r="D39" s="2">
         <v>1959</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="E39" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C40" s="4">
         <v>1846</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D40" s="4">
         <v>1959</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C40" s="2">
-        <v>1846</v>
-      </c>
-      <c r="D40" s="2">
-        <v>1936</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="4" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C41" s="2">
         <v>1846</v>
       </c>
       <c r="D41" s="2">
-        <v>1941</v>
+        <v>1936</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>180</v>
@@ -2171,16 +2186,16 @@
     </row>
     <row r="42" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C42" s="2">
         <v>1846</v>
       </c>
       <c r="D42" s="2">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>180</v>
@@ -2188,16 +2203,16 @@
     </row>
     <row r="43" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C43" s="2">
         <v>1846</v>
       </c>
       <c r="D43" s="2">
-        <v>1981</v>
+        <v>1943</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>180</v>
@@ -2205,33 +2220,33 @@
     </row>
     <row r="44" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" s="2">
+        <v>1846</v>
+      </c>
+      <c r="D44" s="2">
+        <v>1981</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C44" s="2">
-        <v>1847</v>
-      </c>
-      <c r="D44" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="C45" s="2">
         <v>1847</v>
       </c>
       <c r="D45" s="2">
-        <v>1863</v>
+        <v>9999</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>180</v>
@@ -2239,16 +2254,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C46" s="2">
         <v>1847</v>
       </c>
       <c r="D46" s="2">
-        <v>1960</v>
+        <v>1863</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>180</v>
@@ -2256,10 +2271,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C47" s="2">
         <v>1847</v>
@@ -2272,17 +2287,17 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>223</v>
+      <c r="A48" s="5" t="s">
+        <v>220</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C48" s="2">
         <v>1847</v>
       </c>
       <c r="D48" s="2">
-        <v>1980</v>
+        <v>1960</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>180</v>
@@ -2290,10 +2305,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C49" s="2">
         <v>1847</v>
@@ -2307,33 +2322,33 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C50" s="2">
         <v>1847</v>
       </c>
       <c r="D50" s="2">
+        <v>1980</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>225</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="2">
+        <v>1847</v>
+      </c>
+      <c r="D51" s="2">
         <v>1985</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C51" s="2">
-        <v>1848</v>
-      </c>
-      <c r="D51" s="2">
-        <v>1861</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>180</v>
@@ -2341,16 +2356,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C52" s="2">
         <v>1848</v>
       </c>
       <c r="D52" s="2">
-        <v>1972</v>
+        <v>1861</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>180</v>
@@ -2358,16 +2373,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>320</v>
+        <v>222</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C53" s="2">
         <v>1848</v>
       </c>
       <c r="D53" s="2">
-        <v>1981</v>
+        <v>1972</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>180</v>
@@ -2375,16 +2390,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C54" s="2">
         <v>1848</v>
       </c>
       <c r="D54" s="2">
-        <v>2011</v>
+        <v>1981</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>180</v>
@@ -2392,16 +2407,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C55" s="2">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="D55" s="2">
-        <v>9999</v>
+        <v>2011</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>180</v>
@@ -2409,50 +2424,50 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C56" s="2">
         <v>1849</v>
       </c>
       <c r="D56" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="2">
+        <v>1849</v>
+      </c>
+      <c r="D57" s="2">
         <v>1992</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>324</v>
-      </c>
-      <c r="B57" s="1" t="s">
+      <c r="E57" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C57" s="2">
-        <v>1850</v>
-      </c>
-      <c r="D57" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C58" s="2">
         <v>1850</v>
       </c>
       <c r="D58" s="2">
-        <v>1980</v>
+        <v>9999</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>180</v>
@@ -2460,16 +2475,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C59" s="2">
         <v>1850</v>
       </c>
       <c r="D59" s="2">
-        <v>9999</v>
+        <v>1980</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>180</v>
@@ -2477,16 +2492,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C60" s="2">
         <v>1850</v>
       </c>
       <c r="D60" s="2">
-        <v>1993</v>
+        <v>9999</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>180</v>
@@ -2494,16 +2509,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C61" s="2">
         <v>1850</v>
       </c>
       <c r="D61" s="2">
-        <v>1987</v>
+        <v>1993</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>180</v>
@@ -2511,16 +2526,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C62" s="2">
-        <v>1853</v>
+        <v>1850</v>
       </c>
       <c r="D62" s="2">
-        <v>1927</v>
+        <v>1987</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>180</v>
@@ -2528,16 +2543,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C63" s="2">
         <v>1853</v>
       </c>
       <c r="D63" s="2">
-        <v>1958</v>
+        <v>1927</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>180</v>
@@ -2545,84 +2560,84 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" s="2">
+        <v>1853</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1958</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C65" s="2">
         <v>1855</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D65" s="2">
         <v>1981</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+      <c r="E65" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B66" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C65" s="4">
+      <c r="C66" s="4">
         <v>1856</v>
       </c>
-      <c r="D65" s="4">
+      <c r="D66" s="4">
         <v>1912</v>
       </c>
-      <c r="E65" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>308</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="C66" s="4">
+      <c r="E66" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>305</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C67" s="4">
         <v>1857</v>
       </c>
-      <c r="D66" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C67" s="2">
-        <v>1861</v>
-      </c>
-      <c r="D67" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>180</v>
+      <c r="D67" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C68" s="2">
         <v>1861</v>
       </c>
       <c r="D68" s="2">
-        <v>1976</v>
+        <v>9999</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>180</v>
@@ -2630,101 +2645,101 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" s="2">
+        <v>1861</v>
+      </c>
+      <c r="D69" s="2">
+        <v>1976</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C70" s="2">
         <v>1867</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D70" s="2">
         <v>1993</v>
       </c>
-      <c r="E69" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>309</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="C70" s="4">
+      <c r="E70" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>306</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="C71" s="4">
         <v>1868</v>
       </c>
-      <c r="D70" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C71" s="2">
-        <v>1871</v>
-      </c>
-      <c r="D71" s="2">
-        <v>2001</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>180</v>
+      <c r="D71" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C72" s="2">
+        <v>1871</v>
+      </c>
+      <c r="D72" s="2">
+        <v>2001</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C72" s="2">
-        <v>1873</v>
-      </c>
-      <c r="D72" s="2">
-        <v>1993</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C73" s="2">
         <v>1873</v>
       </c>
       <c r="D73" s="2">
+        <v>1993</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1873</v>
+      </c>
+      <c r="D74" s="2">
         <v>1924</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C74" s="2">
-        <v>1874</v>
-      </c>
-      <c r="D74" s="2">
-        <v>1920</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>180</v>
@@ -2732,16 +2747,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C75" s="2">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="D75" s="2">
-        <v>1979</v>
+        <v>1920</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>180</v>
@@ -2749,169 +2764,169 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C76" s="2">
+        <v>1875</v>
+      </c>
+      <c r="D76" s="2">
+        <v>1979</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C77" s="2">
         <v>1886</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D77" s="2">
         <v>1961</v>
       </c>
-      <c r="E76" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C77" s="2">
-        <v>1889</v>
-      </c>
-      <c r="D77" s="2">
-        <v>9999</v>
-      </c>
       <c r="E77" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>235</v>
+        <v>362</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>60</v>
+        <v>363</v>
       </c>
       <c r="C78" s="2">
-        <v>1894</v>
+        <v>1888</v>
       </c>
       <c r="D78" s="2">
-        <v>1919</v>
+        <v>9999</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>235</v>
+      <c r="A79" s="7" t="s">
+        <v>315</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C79" s="2">
-        <v>1894</v>
+        <v>1889</v>
       </c>
       <c r="D79" s="2">
         <v>9999</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>338</v>
+        <v>235</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C80" s="2">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="D80" s="2">
-        <v>9999</v>
+        <v>1919</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>319</v>
+        <v>235</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C81" s="2">
-        <v>1898</v>
+        <v>1894</v>
       </c>
       <c r="D81" s="2">
         <v>9999</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>235</v>
+        <v>335</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C82" s="2">
-        <v>1899</v>
+        <v>1897</v>
       </c>
       <c r="D82" s="2">
         <v>9999</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>226</v>
+      <c r="A83" s="5" t="s">
+        <v>316</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C83" s="2">
-        <v>1901</v>
+        <v>1898</v>
       </c>
       <c r="D83" s="2">
-        <v>1987</v>
+        <v>9999</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>227</v>
+      <c r="A84" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C84" s="2">
-        <v>1901</v>
+        <v>1899</v>
       </c>
       <c r="D84" s="2">
-        <v>1938</v>
+        <v>9999</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>228</v>
+      <c r="A85" t="s">
+        <v>226</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C85" s="2">
         <v>1901</v>
       </c>
       <c r="D85" s="2">
-        <v>9999</v>
+        <v>1987</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>179</v>
@@ -2919,16 +2934,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C86" s="2">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="D86" s="2">
-        <v>9999</v>
+        <v>1938</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>179</v>
@@ -2936,13 +2951,13 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>339</v>
+        <v>228</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C87" s="2">
-        <v>1906</v>
+        <v>1901</v>
       </c>
       <c r="D87" s="2">
         <v>9999</v>
@@ -2952,14 +2967,14 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>340</v>
+      <c r="A88" t="s">
+        <v>229</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C88" s="2">
-        <v>1907</v>
+        <v>1904</v>
       </c>
       <c r="D88" s="2">
         <v>9999</v>
@@ -2969,31 +2984,31 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>230</v>
+      <c r="A89" s="5" t="s">
+        <v>336</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C89" s="2">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="D89" s="2">
-        <v>1987</v>
+        <v>9999</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>299</v>
+      <c r="A90" s="5" t="s">
+        <v>337</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C90" s="2">
-        <v>1912</v>
+        <v>1907</v>
       </c>
       <c r="D90" s="2">
         <v>9999</v>
@@ -3004,30 +3019,30 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C91" s="2">
-        <v>1912</v>
+        <v>1908</v>
       </c>
       <c r="D91" s="2">
-        <v>9999</v>
+        <v>1987</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>232</v>
+      <c r="A92" t="s">
+        <v>296</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C92" s="2">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="D92" s="2">
         <v>9999</v>
@@ -3037,14 +3052,14 @@
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>233</v>
+      <c r="A93" t="s">
+        <v>231</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C93" s="2">
-        <v>1915</v>
+        <v>1912</v>
       </c>
       <c r="D93" s="2">
         <v>9999</v>
@@ -3055,13 +3070,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C94" s="2">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="D94" s="2">
         <v>9999</v>
@@ -3072,13 +3087,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>347</v>
+        <v>233</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C95" s="2">
-        <v>1917</v>
+        <v>1915</v>
       </c>
       <c r="D95" s="2">
         <v>9999</v>
@@ -3089,13 +3104,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>348</v>
+        <v>234</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C96" s="2">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="D96" s="2">
         <v>9999</v>
@@ -3106,33 +3121,33 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>235</v>
+        <v>344</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C97" s="2">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="D97" s="2">
-        <v>2009</v>
+        <v>9999</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>236</v>
+      <c r="A98" s="5" t="s">
+        <v>345</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C98" s="2">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="D98" s="2">
-        <v>1975</v>
+        <v>9999</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>179</v>
@@ -3143,44 +3158,44 @@
         <v>235</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C99" s="2">
-        <v>1922</v>
+        <v>1919</v>
       </c>
       <c r="D99" s="2">
-        <v>9999</v>
+        <v>2009</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C100" s="2">
-        <v>1923</v>
+        <v>1919</v>
       </c>
       <c r="D100" s="2">
-        <v>9999</v>
+        <v>1975</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C101" s="2">
-        <v>1927</v>
+        <v>1922</v>
       </c>
       <c r="D101" s="2">
         <v>9999</v>
@@ -3190,31 +3205,31 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>239</v>
+      <c r="A102" t="s">
+        <v>237</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C102" s="2">
-        <v>1928</v>
+        <v>1923</v>
       </c>
       <c r="D102" s="2">
         <v>9999</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>240</v>
+        <v>365</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C103" s="2">
-        <v>1929</v>
+        <v>1927</v>
       </c>
       <c r="D103" s="2">
         <v>9999</v>
@@ -3225,81 +3240,81 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>241</v>
+        <v>366</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C104" s="2">
-        <v>1934</v>
+        <v>1928</v>
       </c>
       <c r="D104" s="2">
         <v>9999</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>235</v>
+        <v>364</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C105" s="2">
-        <v>1936</v>
+        <v>1929</v>
       </c>
       <c r="D105" s="2">
-        <v>1963</v>
+        <v>9999</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>243</v>
+      <c r="A106" s="5" t="s">
+        <v>238</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C106" s="2">
-        <v>1941</v>
+        <v>1934</v>
       </c>
       <c r="D106" s="2">
         <v>9999</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C107" s="2">
-        <v>1941</v>
+        <v>1936</v>
       </c>
       <c r="D107" s="2">
-        <v>9999</v>
+        <v>1963</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>235</v>
+      <c r="A108" t="s">
+        <v>240</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C108" s="2">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="D108" s="2">
         <v>9999</v>
@@ -3310,16 +3325,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C109" s="2">
-        <v>1947</v>
+        <v>1941</v>
       </c>
       <c r="D109" s="2">
-        <v>1964</v>
+        <v>9999</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>179</v>
@@ -3327,78 +3342,78 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B110" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C110" s="2">
+        <v>1943</v>
+      </c>
+      <c r="D110" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C111" s="2">
+        <v>1947</v>
+      </c>
+      <c r="D111" s="2">
+        <v>1964</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C110" s="2">
+      <c r="C112" s="2">
         <v>1950</v>
       </c>
-      <c r="D110" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>245</v>
-      </c>
-      <c r="B111" s="1" t="s">
+      <c r="D112" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>242</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C111" s="2">
+      <c r="C113" s="2">
         <v>1951</v>
       </c>
-      <c r="D111" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>310</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="C112" s="2">
-        <v>1952</v>
-      </c>
-      <c r="D112" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C113" s="2">
-        <v>1952</v>
-      </c>
       <c r="D113" s="2">
-        <v>2009</v>
+        <v>9999</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>246</v>
+      <c r="A114" t="s">
+        <v>307</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>94</v>
+        <v>308</v>
       </c>
       <c r="C114" s="2">
         <v>1952</v>
@@ -3407,21 +3422,21 @@
         <v>9999</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C115" s="2">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="D115" s="2">
-        <v>9999</v>
+        <v>2009</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>177</v>
@@ -3429,27 +3444,27 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C116" s="2">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="D116" s="2">
         <v>9999</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C117" s="2">
         <v>1954</v>
@@ -3458,18 +3473,18 @@
         <v>9999</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C118" s="2">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="D118" s="2">
         <v>9999</v>
@@ -3480,33 +3495,33 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C119" s="2">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="D119" s="2">
         <v>9999</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>171</v>
+        <v>99</v>
       </c>
       <c r="C120" s="2">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="D120" s="2">
-        <v>2016</v>
+        <v>9999</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>177</v>
@@ -3514,33 +3529,33 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>351</v>
+        <v>235</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C121" s="2">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="D121" s="2">
         <v>9999</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>300</v>
+        <v>235</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>101</v>
+        <v>171</v>
       </c>
       <c r="C122" s="2">
         <v>1957</v>
       </c>
       <c r="D122" s="2">
-        <v>9999</v>
+        <v>2016</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>177</v>
@@ -3548,13 +3563,13 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>312</v>
+        <v>358</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C123" s="2">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="D123" s="2">
         <v>9999</v>
@@ -3563,29 +3578,29 @@
         <v>177</v>
       </c>
     </row>
-    <row r="124" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>350</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C124" s="4">
-        <v>1958</v>
-      </c>
-      <c r="D124" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E124" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C124" s="2">
+        <v>1957</v>
+      </c>
+      <c r="D124" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E124" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>251</v>
+        <v>309</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C125" s="2">
         <v>1958</v>
@@ -3597,32 +3612,32 @@
         <v>177</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C126" s="2">
-        <v>1959</v>
-      </c>
-      <c r="D126" s="2">
-        <v>2004</v>
-      </c>
-      <c r="E126" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C126" s="4">
+        <v>1958</v>
+      </c>
+      <c r="D126" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E126" s="4" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>169</v>
+        <v>105</v>
       </c>
       <c r="C127" s="2">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="D127" s="2">
         <v>9999</v>
@@ -3633,78 +3648,78 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>106</v>
+        <v>170</v>
       </c>
       <c r="C128" s="2">
         <v>1959</v>
       </c>
       <c r="D128" s="2">
-        <v>9999</v>
+        <v>2004</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="B129" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C129" s="4">
-        <v>1961</v>
-      </c>
-      <c r="D129" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E129" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C129" s="2">
+        <v>1959</v>
+      </c>
+      <c r="D129" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E129" s="2" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C130" s="2">
-        <v>1962</v>
+        <v>1959</v>
       </c>
       <c r="D130" s="2">
         <v>9999</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>298</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C131" s="2">
-        <v>1962</v>
-      </c>
-      <c r="D131" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E131" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C131" s="4">
+        <v>1961</v>
+      </c>
+      <c r="D131" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E131" s="4" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C132" s="2">
         <v>1962</v>
@@ -3717,14 +3732,14 @@
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="5" t="s">
-        <v>349</v>
+      <c r="A133" t="s">
+        <v>295</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>110</v>
+        <v>252</v>
       </c>
       <c r="C133" s="2">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="D133" s="2">
         <v>9999</v>
@@ -3734,14 +3749,14 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>313</v>
+      <c r="A134" s="5" t="s">
+        <v>251</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C134" s="2">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="D134" s="2">
         <v>9999</v>
@@ -3752,13 +3767,13 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>314</v>
+        <v>346</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C135" s="2">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="D135" s="2">
         <v>9999</v>
@@ -3768,11 +3783,11 @@
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="5" t="s">
-        <v>235</v>
+      <c r="A136" t="s">
+        <v>310</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C136" s="2">
         <v>1964</v>
@@ -3781,46 +3796,49 @@
         <v>9999</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B137" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C137" s="2">
+        <v>1964</v>
+      </c>
+      <c r="D137" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C138" s="2">
+        <v>1964</v>
+      </c>
+      <c r="D138" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="C137" s="2">
-        <v>1965</v>
-      </c>
-      <c r="D137" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E137" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B138" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C138" s="2">
-        <v>1965</v>
-      </c>
-      <c r="D138" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>297</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="C139" s="2">
         <v>1965</v>
@@ -3833,14 +3851,11 @@
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>296</v>
-      </c>
       <c r="B140" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C140" s="2">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="D140" s="2">
         <v>9999</v>
@@ -3851,146 +3866,146 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C141" s="2">
+        <v>1965</v>
+      </c>
+      <c r="D141" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>293</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C142" s="2">
+        <v>1966</v>
+      </c>
+      <c r="D142" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>292</v>
+      </c>
+      <c r="B143" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C141" s="2">
+      <c r="C143" s="2">
         <v>1969</v>
       </c>
-      <c r="D141" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E141" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="B142" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="C142" s="4">
+      <c r="D143" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C144" s="4">
         <v>1970</v>
       </c>
-      <c r="D142" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E142" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C143" s="2">
-        <v>1971</v>
-      </c>
-      <c r="D143" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>293</v>
-      </c>
-      <c r="B144" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C144" s="2">
-        <v>1973</v>
-      </c>
-      <c r="D144" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E144" s="2" t="s">
+      <c r="D144" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E144" s="4" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>235</v>
+        <v>291</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C145" s="2">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="D145" s="2">
         <v>9999</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C146" s="2">
-        <v>1975</v>
+        <v>1973</v>
       </c>
       <c r="D146" s="2">
         <v>9999</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B147" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C147" s="4">
+      <c r="B147" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C147" s="2">
+        <v>1974</v>
+      </c>
+      <c r="D147" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>289</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C148" s="2">
         <v>1975</v>
       </c>
-      <c r="D147" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E147" s="4" t="s">
+      <c r="D148" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E148" s="2" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="B148" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C148" s="4">
-        <v>1975</v>
-      </c>
-      <c r="D148" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E148" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="149" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>290</v>
+        <v>235</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>361</v>
+        <v>140</v>
       </c>
       <c r="C149" s="4">
         <v>1975</v>
@@ -3999,35 +4014,35 @@
         <v>9999</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C150" s="2">
-        <v>1979</v>
-      </c>
-      <c r="D150" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E150" s="2" t="s">
-        <v>180</v>
+      <c r="B150" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C150" s="4">
+        <v>1975</v>
+      </c>
+      <c r="D150" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="151" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>289</v>
+        <v>357</v>
       </c>
       <c r="C151" s="4">
-        <v>1980</v>
+        <v>1975</v>
       </c>
       <c r="D151" s="4">
         <v>9999</v>
@@ -4038,35 +4053,35 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C152" s="2">
-        <v>1984</v>
+        <v>1979</v>
       </c>
       <c r="D152" s="2">
         <v>9999</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C153" s="2">
-        <v>1985</v>
-      </c>
-      <c r="D153" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E153" s="2" t="s">
+      <c r="B153" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C153" s="4">
+        <v>1980</v>
+      </c>
+      <c r="D153" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E153" s="4" t="s">
         <v>179</v>
       </c>
     </row>
@@ -4075,27 +4090,27 @@
         <v>283</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C154" s="2">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="D154" s="2">
         <v>9999</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C155" s="2">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="D155" s="2">
         <v>9999</v>
@@ -4106,13 +4121,13 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C156" s="2">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="D156" s="2">
         <v>9999</v>
@@ -4126,67 +4141,67 @@
         <v>281</v>
       </c>
       <c r="B157" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C157" s="2">
+        <v>1987</v>
+      </c>
+      <c r="D157" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C158" s="2">
+        <v>1992</v>
+      </c>
+      <c r="D158" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B159" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C157" s="2">
+      <c r="C159" s="2">
         <v>1992</v>
       </c>
-      <c r="D157" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E157" s="2" t="s">
+      <c r="D159" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E159" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="158" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="5" t="s">
+    <row r="160" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B158" s="5" t="s">
+      <c r="B160" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C158" s="4">
+      <c r="C160" s="4">
         <v>1993</v>
       </c>
-      <c r="D158" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E158" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C159" s="4">
-        <v>1994</v>
-      </c>
-      <c r="D159" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E159" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>301</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C160" s="2">
-        <v>1994</v>
-      </c>
-      <c r="D160" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>180</v>
+      <c r="D160" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E160" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="161" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4194,10 +4209,10 @@
         <v>235</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C161" s="4">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D161" s="4">
         <v>9999</v>
@@ -4207,147 +4222,147 @@
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="5" t="s">
-        <v>280</v>
+      <c r="A162" t="s">
+        <v>298</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C162" s="2">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="D162" s="2">
         <v>9999</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B163" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C163" s="2">
+      <c r="B163" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C163" s="4">
         <v>1995</v>
       </c>
-      <c r="D163" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E163" s="2" t="s">
-        <v>179</v>
+      <c r="D163" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E163" s="4" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C164" s="2">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="D164" s="2">
         <v>9999</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B165" s="5" t="s">
+      <c r="B165" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C165" s="2">
+        <v>1995</v>
+      </c>
+      <c r="D165" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C166" s="2">
+        <v>1997</v>
+      </c>
+      <c r="D166" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B167" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C165" s="4">
+      <c r="C167" s="4">
         <v>1998</v>
       </c>
-      <c r="D165" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E165" s="4" t="s">
+      <c r="D167" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E167" s="4" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>278</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C166" s="2">
-        <v>1998</v>
-      </c>
-      <c r="D166" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>276</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C167" s="2">
-        <v>1999</v>
-      </c>
-      <c r="D167" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C168" s="2">
-        <v>2002</v>
+        <v>1998</v>
       </c>
       <c r="D168" s="2">
         <v>9999</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B169" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C169" s="4">
-        <v>2002</v>
-      </c>
-      <c r="D169" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E169" s="4" t="s">
-        <v>177</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>273</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C169" s="2">
+        <v>1999</v>
+      </c>
+      <c r="D169" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C170" s="2">
         <v>2002</v>
@@ -4356,49 +4371,49 @@
         <v>9999</v>
       </c>
       <c r="E170" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C171" s="4">
+        <v>2002</v>
+      </c>
+      <c r="D171" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E171" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>272</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C172" s="2">
+        <v>2002</v>
+      </c>
+      <c r="D172" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E172" s="2" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>274</v>
-      </c>
-      <c r="B171" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C171" s="2">
-        <v>2003</v>
-      </c>
-      <c r="D171" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E171" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B172" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C172" s="4">
-        <v>2003</v>
-      </c>
-      <c r="D172" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E172" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C173" s="2">
         <v>2003</v>
@@ -4407,49 +4422,49 @@
         <v>9999</v>
       </c>
       <c r="E173" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C174" s="4">
+        <v>2003</v>
+      </c>
+      <c r="D174" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E174" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>270</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C175" s="2">
+        <v>2003</v>
+      </c>
+      <c r="D175" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E175" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>272</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="C174" s="2">
-        <v>2005</v>
-      </c>
-      <c r="D174" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E174" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C175" s="2">
-        <v>2005</v>
-      </c>
-      <c r="D175" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E175" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="5" t="s">
-        <v>235</v>
+      <c r="A176" t="s">
+        <v>269</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>147</v>
+        <v>351</v>
       </c>
       <c r="C176" s="2">
         <v>2005</v>
@@ -4458,69 +4473,69 @@
         <v>9999</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>271</v>
+      <c r="A177" s="5" t="s">
+        <v>235</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>354</v>
+        <v>148</v>
       </c>
       <c r="C177" s="2">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="D177" s="2">
         <v>9999</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
       <c r="B178" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C178" s="2">
+        <v>2005</v>
+      </c>
+      <c r="D178" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>268</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C179" s="2">
+        <v>2006</v>
+      </c>
+      <c r="D179" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B180" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C178" s="2">
+      <c r="C180" s="2">
         <v>2007</v>
-      </c>
-      <c r="D178" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E178" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C179" s="2">
-        <v>2007</v>
-      </c>
-      <c r="D179" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E179" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>264</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C180" s="2">
-        <v>2008</v>
       </c>
       <c r="D180" s="2">
         <v>9999</v>
@@ -4529,21 +4544,21 @@
         <v>183</v>
       </c>
     </row>
-    <row r="181" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B181" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C181" s="4">
-        <v>2008</v>
-      </c>
-      <c r="D181" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E181" s="4" t="s">
-        <v>183</v>
+        <v>348</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C181" s="2">
+        <v>2007</v>
+      </c>
+      <c r="D181" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -4551,10 +4566,10 @@
         <v>261</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C182" s="2">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="D182" s="2">
         <v>9999</v>
@@ -4563,29 +4578,29 @@
         <v>183</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B183" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C183" s="2">
-        <v>2009</v>
-      </c>
-      <c r="D183" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>181</v>
+      <c r="B183" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C183" s="4">
+        <v>2008</v>
+      </c>
+      <c r="D183" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E183" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C184" s="2">
         <v>2009</v>
@@ -4594,57 +4609,57 @@
         <v>9999</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B185" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C185" s="4">
-        <v>2010</v>
-      </c>
-      <c r="D185" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E185" s="4" t="s">
-        <v>183</v>
+      <c r="B185" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C185" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D185" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C186" s="2">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="D186" s="2">
         <v>9999</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="B187" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C187" s="2">
-        <v>2012</v>
-      </c>
-      <c r="D187" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E187" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C187" s="4">
+        <v>2010</v>
+      </c>
+      <c r="D187" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E187" s="4" t="s">
         <v>183</v>
       </c>
     </row>
@@ -4653,10 +4668,10 @@
         <v>260</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C188" s="2">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D188" s="2">
         <v>9999</v>
@@ -4666,14 +4681,14 @@
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>265</v>
+      <c r="A189" s="5" t="s">
+        <v>266</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C189" s="2">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D189" s="2">
         <v>9999</v>
@@ -4682,32 +4697,32 @@
         <v>183</v>
       </c>
     </row>
-    <row r="190" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B190" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C190" s="4">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>257</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C190" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D190" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>262</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C191" s="2">
         <v>2014</v>
-      </c>
-      <c r="D190" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E190" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C191" s="2">
-        <v>2015</v>
       </c>
       <c r="D191" s="2">
         <v>9999</v>
@@ -4716,29 +4731,29 @@
         <v>183</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>267</v>
-      </c>
-      <c r="B192" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C192" s="2">
-        <v>2015</v>
-      </c>
-      <c r="D192" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E192" s="2" t="s">
-        <v>183</v>
+    <row r="192" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C192" s="4">
+        <v>2014</v>
+      </c>
+      <c r="D192" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E192" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>268</v>
+      <c r="A193" s="5" t="s">
+        <v>263</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C193" s="2">
         <v>2015</v>
@@ -4750,100 +4765,100 @@
         <v>183</v>
       </c>
     </row>
-    <row r="194" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="5" t="s">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>264</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C194" s="2">
+        <v>2015</v>
+      </c>
+      <c r="D194" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E194" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>265</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C195" s="2">
+        <v>2015</v>
+      </c>
+      <c r="D195" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E195" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B194" s="5" t="s">
+      <c r="B196" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C194" s="4">
+      <c r="C196" s="4">
         <v>2016</v>
       </c>
-      <c r="D194" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E194" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="5" t="s">
+      <c r="D196" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E196" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B195" s="5" t="s">
+      <c r="B197" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C195" s="4">
+      <c r="C197" s="4">
         <v>2017</v>
       </c>
-      <c r="D195" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E195" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="B196" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="C196" s="4">
+      <c r="D197" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E197" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C198" s="4">
         <v>2018</v>
       </c>
-      <c r="D196" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E196" s="4" t="s">
+      <c r="D198" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E198" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B197" s="1" t="s">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B199" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C197" s="2">
+      <c r="C199" s="2">
         <v>2018</v>
-      </c>
-      <c r="D197" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E197" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>259</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C198" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D198" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E198" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>257</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C199" s="2">
-        <v>2019</v>
       </c>
       <c r="D199" s="2">
         <v>9999</v>
@@ -4857,10 +4872,10 @@
         <v>256</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C200" s="2">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="D200" s="2">
         <v>9999</v>
@@ -4869,10 +4884,44 @@
         <v>179</v>
       </c>
     </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>254</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C201" s="2">
+        <v>2019</v>
+      </c>
+      <c r="D201" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E201" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>253</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C202" s="2">
+        <v>2021</v>
+      </c>
+      <c r="D202" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E200">
-    <sortCondition ref="C2:C200"/>
-    <sortCondition ref="E2:E200"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E202">
+    <sortCondition ref="C2:C202"/>
+    <sortCondition ref="E2:E202"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed name of "event" column to "milestone".
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\prototype-historical-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B43E6ED-CFF5-4FC1-8BC8-F5B3B69BA710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3AA8E5-5040-4D28-9B56-76F83C486D52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{48B35B47-D791-4DB0-8E3F-11AF1DC17D23}"/>
   </bookViews>
@@ -552,9 +552,6 @@
     <t>end_year</t>
   </si>
   <si>
-    <t>event</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -1126,6 +1123,9 @@
   </si>
   <si>
     <t>Red_Line-1928</t>
+  </si>
+  <si>
+    <t>milestone</t>
   </si>
 </sst>
 </file>
@@ -1504,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB246BE0-9101-4910-B137-94A0FD6048BC}">
   <dimension ref="A1:E202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,10 +1519,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>175</v>
+        <v>366</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>173</v>
@@ -1531,12 +1531,12 @@
         <v>174</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -1545,12 +1545,12 @@
         <v>9999</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -1559,12 +1559,12 @@
         <v>9999</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -1573,12 +1573,12 @@
         <v>9999</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -1587,12 +1587,12 @@
         <v>9999</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -1601,12 +1601,12 @@
         <v>9999</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -1615,12 +1615,12 @@
         <v>9999</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -1629,12 +1629,12 @@
         <v>9999</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -1643,12 +1643,12 @@
         <v>9999</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -1657,12 +1657,12 @@
         <v>9999</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="2">
         <v>0</v>
@@ -1671,12 +1671,12 @@
         <v>9999</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>0</v>
@@ -1688,12 +1688,12 @@
         <v>1868</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
@@ -1705,12 +1705,12 @@
         <v>1838</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
@@ -1722,12 +1722,12 @@
         <v>9999</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -1739,12 +1739,12 @@
         <v>1857</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
@@ -1756,12 +1756,12 @@
         <v>1829</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>5</v>
@@ -1773,12 +1773,12 @@
         <v>1845</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -1790,12 +1790,12 @@
         <v>1830</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
@@ -1807,12 +1807,12 @@
         <v>1841</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>8</v>
@@ -1824,12 +1824,12 @@
         <v>9999</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>9</v>
@@ -1841,12 +1841,12 @@
         <v>9999</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>11</v>
@@ -1858,12 +1858,12 @@
         <v>1849</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>10</v>
@@ -1875,15 +1875,15 @@
         <v>1871</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C24" s="4">
         <v>1829</v>
@@ -1892,15 +1892,15 @@
         <v>9999</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B25" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C25" s="4">
         <v>1830</v>
@@ -1909,12 +1909,12 @@
         <v>9999</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>12</v>
@@ -1926,15 +1926,15 @@
         <v>9999</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="C27" s="2">
         <v>1834</v>
@@ -1943,12 +1943,12 @@
         <v>9999</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>13</v>
@@ -1960,12 +1960,12 @@
         <v>9999</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>14</v>
@@ -1977,15 +1977,15 @@
         <v>9999</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C30" s="4">
         <v>1838</v>
@@ -1994,12 +1994,12 @@
         <v>9999</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>15</v>
@@ -2011,12 +2011,12 @@
         <v>9999</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>16</v>
@@ -2028,12 +2028,12 @@
         <v>1976</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>17</v>
@@ -2045,12 +2045,12 @@
         <v>9999</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>18</v>
@@ -2062,12 +2062,12 @@
         <v>1961</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>19</v>
@@ -2079,12 +2079,12 @@
         <v>9999</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>20</v>
@@ -2096,15 +2096,15 @@
         <v>1966</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C37" s="4">
         <v>1845</v>
@@ -2113,12 +2113,12 @@
         <v>9999</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>21</v>
@@ -2130,12 +2130,12 @@
         <v>9999</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>22</v>
@@ -2147,12 +2147,12 @@
         <v>1959</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>23</v>
@@ -2164,12 +2164,12 @@
         <v>1959</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>27</v>
@@ -2181,12 +2181,12 @@
         <v>1936</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>26</v>
@@ -2198,12 +2198,12 @@
         <v>1941</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>25</v>
@@ -2215,12 +2215,12 @@
         <v>1943</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>24</v>
@@ -2232,12 +2232,12 @@
         <v>1981</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>34</v>
@@ -2249,12 +2249,12 @@
         <v>9999</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>33</v>
@@ -2266,12 +2266,12 @@
         <v>1863</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>32</v>
@@ -2283,12 +2283,12 @@
         <v>1960</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>31</v>
@@ -2300,12 +2300,12 @@
         <v>1960</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>30</v>
@@ -2317,12 +2317,12 @@
         <v>1980</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>29</v>
@@ -2334,12 +2334,12 @@
         <v>1980</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>28</v>
@@ -2351,12 +2351,12 @@
         <v>1985</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>35</v>
@@ -2368,12 +2368,12 @@
         <v>1861</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>36</v>
@@ -2385,12 +2385,12 @@
         <v>1972</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>37</v>
@@ -2402,12 +2402,12 @@
         <v>1981</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>38</v>
@@ -2419,12 +2419,12 @@
         <v>2011</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>40</v>
@@ -2436,12 +2436,12 @@
         <v>9999</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>39</v>
@@ -2453,12 +2453,12 @@
         <v>1992</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>41</v>
@@ -2470,12 +2470,12 @@
         <v>9999</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>42</v>
@@ -2487,12 +2487,12 @@
         <v>1980</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>43</v>
@@ -2504,12 +2504,12 @@
         <v>9999</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>44</v>
@@ -2521,12 +2521,12 @@
         <v>1993</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>45</v>
@@ -2538,12 +2538,12 @@
         <v>1987</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>47</v>
@@ -2555,12 +2555,12 @@
         <v>1927</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>46</v>
@@ -2572,12 +2572,12 @@
         <v>1958</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>48</v>
@@ -2589,12 +2589,12 @@
         <v>1981</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>49</v>
@@ -2606,15 +2606,15 @@
         <v>1912</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C67" s="4">
         <v>1857</v>
@@ -2623,12 +2623,12 @@
         <v>9999</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>50</v>
@@ -2640,12 +2640,12 @@
         <v>9999</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>51</v>
@@ -2657,12 +2657,12 @@
         <v>1976</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>52</v>
@@ -2674,15 +2674,15 @@
         <v>1993</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C71" s="4">
         <v>1868</v>
@@ -2691,12 +2691,12 @@
         <v>9999</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>53</v>
@@ -2708,12 +2708,12 @@
         <v>2001</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>54</v>
@@ -2725,12 +2725,12 @@
         <v>1993</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="74" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>55</v>
@@ -2742,12 +2742,12 @@
         <v>1924</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>56</v>
@@ -2759,12 +2759,12 @@
         <v>1920</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>57</v>
@@ -2776,12 +2776,12 @@
         <v>1979</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>58</v>
@@ -2793,15 +2793,15 @@
         <v>1961</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>363</v>
       </c>
       <c r="C78" s="2">
         <v>1888</v>
@@ -2810,12 +2810,12 @@
         <v>9999</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>59</v>
@@ -2827,12 +2827,12 @@
         <v>9999</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>60</v>
@@ -2844,12 +2844,12 @@
         <v>1919</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>61</v>
@@ -2861,12 +2861,12 @@
         <v>9999</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>62</v>
@@ -2878,12 +2878,12 @@
         <v>9999</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>63</v>
@@ -2895,12 +2895,12 @@
         <v>9999</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>64</v>
@@ -2912,12 +2912,12 @@
         <v>9999</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>66</v>
@@ -2929,12 +2929,12 @@
         <v>1987</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>65</v>
@@ -2946,12 +2946,12 @@
         <v>1938</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>67</v>
@@ -2963,12 +2963,12 @@
         <v>9999</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>68</v>
@@ -2980,12 +2980,12 @@
         <v>9999</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>69</v>
@@ -2997,12 +2997,12 @@
         <v>9999</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>70</v>
@@ -3014,12 +3014,12 @@
         <v>9999</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>71</v>
@@ -3031,12 +3031,12 @@
         <v>1987</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>72</v>
@@ -3048,12 +3048,12 @@
         <v>9999</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>73</v>
@@ -3065,12 +3065,12 @@
         <v>9999</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>74</v>
@@ -3082,12 +3082,12 @@
         <v>9999</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>75</v>
@@ -3099,12 +3099,12 @@
         <v>9999</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>76</v>
@@ -3116,12 +3116,12 @@
         <v>9999</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>77</v>
@@ -3133,12 +3133,12 @@
         <v>9999</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>78</v>
@@ -3150,12 +3150,12 @@
         <v>9999</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>79</v>
@@ -3167,12 +3167,12 @@
         <v>2009</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>80</v>
@@ -3184,12 +3184,12 @@
         <v>1975</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>81</v>
@@ -3201,12 +3201,12 @@
         <v>9999</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>83</v>
@@ -3218,12 +3218,12 @@
         <v>9999</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>82</v>
@@ -3235,12 +3235,12 @@
         <v>9999</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>84</v>
@@ -3252,12 +3252,12 @@
         <v>9999</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>85</v>
@@ -3269,12 +3269,12 @@
         <v>9999</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>87</v>
@@ -3286,12 +3286,12 @@
         <v>9999</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>86</v>
@@ -3303,12 +3303,12 @@
         <v>1963</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>89</v>
@@ -3320,12 +3320,12 @@
         <v>9999</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>88</v>
@@ -3337,12 +3337,12 @@
         <v>9999</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>90</v>
@@ -3354,12 +3354,12 @@
         <v>9999</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>91</v>
@@ -3371,12 +3371,12 @@
         <v>1964</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>92</v>
@@ -3388,12 +3388,12 @@
         <v>9999</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>93</v>
@@ -3405,15 +3405,15 @@
         <v>9999</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>306</v>
+      </c>
+      <c r="B114" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>308</v>
       </c>
       <c r="C114" s="2">
         <v>1952</v>
@@ -3422,12 +3422,12 @@
         <v>9999</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>95</v>
@@ -3439,12 +3439,12 @@
         <v>2009</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>94</v>
@@ -3456,12 +3456,12 @@
         <v>9999</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>97</v>
@@ -3473,12 +3473,12 @@
         <v>9999</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>98</v>
@@ -3490,12 +3490,12 @@
         <v>9999</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>96</v>
@@ -3507,12 +3507,12 @@
         <v>9999</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>99</v>
@@ -3524,12 +3524,12 @@
         <v>9999</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>100</v>
@@ -3541,12 +3541,12 @@
         <v>9999</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>171</v>
@@ -3558,12 +3558,12 @@
         <v>2016</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>102</v>
@@ -3575,12 +3575,12 @@
         <v>9999</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>101</v>
@@ -3592,12 +3592,12 @@
         <v>9999</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>103</v>
@@ -3609,12 +3609,12 @@
         <v>9999</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="126" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>104</v>
@@ -3626,12 +3626,12 @@
         <v>9999</v>
       </c>
       <c r="E126" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>105</v>
@@ -3643,12 +3643,12 @@
         <v>9999</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>170</v>
@@ -3660,12 +3660,12 @@
         <v>2004</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>169</v>
@@ -3677,12 +3677,12 @@
         <v>9999</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>106</v>
@@ -3694,12 +3694,12 @@
         <v>9999</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="131" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>107</v>
@@ -3711,12 +3711,12 @@
         <v>9999</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>108</v>
@@ -3728,15 +3728,15 @@
         <v>9999</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C133" s="2">
         <v>1962</v>
@@ -3745,12 +3745,12 @@
         <v>9999</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>109</v>
@@ -3762,12 +3762,12 @@
         <v>9999</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>110</v>
@@ -3779,12 +3779,12 @@
         <v>9999</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>112</v>
@@ -3796,12 +3796,12 @@
         <v>9999</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>113</v>
@@ -3813,12 +3813,12 @@
         <v>9999</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>111</v>
@@ -3830,12 +3830,12 @@
         <v>9999</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>114</v>
@@ -3847,7 +3847,7 @@
         <v>9999</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3861,12 +3861,12 @@
         <v>9999</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>115</v>
@@ -3878,12 +3878,12 @@
         <v>9999</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>117</v>
@@ -3895,12 +3895,12 @@
         <v>9999</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>118</v>
@@ -3912,15 +3912,15 @@
         <v>9999</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="144" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B144" s="5" t="s">
         <v>313</v>
-      </c>
-      <c r="B144" s="5" t="s">
-        <v>314</v>
       </c>
       <c r="C144" s="4">
         <v>1970</v>
@@ -3929,12 +3929,12 @@
         <v>9999</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>119</v>
@@ -3946,12 +3946,12 @@
         <v>9999</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>120</v>
@@ -3963,12 +3963,12 @@
         <v>9999</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>121</v>
@@ -3980,12 +3980,12 @@
         <v>9999</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>139</v>
@@ -3997,12 +3997,12 @@
         <v>9999</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="149" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>140</v>
@@ -4014,15 +4014,15 @@
         <v>9999</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="150" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B150" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="B150" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="C150" s="4">
         <v>1975</v>
@@ -4031,15 +4031,15 @@
         <v>9999</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="151" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C151" s="4">
         <v>1975</v>
@@ -4048,12 +4048,12 @@
         <v>9999</v>
       </c>
       <c r="E151" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>122</v>
@@ -4065,15 +4065,15 @@
         <v>9999</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="153" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B153" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="B153" s="5" t="s">
-        <v>286</v>
       </c>
       <c r="C153" s="4">
         <v>1980</v>
@@ -4082,12 +4082,12 @@
         <v>9999</v>
       </c>
       <c r="E153" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>123</v>
@@ -4099,12 +4099,12 @@
         <v>9999</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>124</v>
@@ -4116,12 +4116,12 @@
         <v>9999</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>141</v>
@@ -4133,12 +4133,12 @@
         <v>9999</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>125</v>
@@ -4150,12 +4150,12 @@
         <v>9999</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>142</v>
@@ -4167,12 +4167,12 @@
         <v>9999</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>143</v>
@@ -4184,12 +4184,12 @@
         <v>9999</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="160" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B160" s="5" t="s">
         <v>126</v>
@@ -4201,12 +4201,12 @@
         <v>9999</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="161" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B161" s="5" t="s">
         <v>127</v>
@@ -4218,12 +4218,12 @@
         <v>9999</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>128</v>
@@ -4235,12 +4235,12 @@
         <v>9999</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="163" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B163" s="5" t="s">
         <v>130</v>
@@ -4252,12 +4252,12 @@
         <v>9999</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>131</v>
@@ -4269,12 +4269,12 @@
         <v>9999</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>129</v>
@@ -4286,12 +4286,12 @@
         <v>9999</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>132</v>
@@ -4303,12 +4303,12 @@
         <v>9999</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="167" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>134</v>
@@ -4320,12 +4320,12 @@
         <v>9999</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>133</v>
@@ -4337,12 +4337,12 @@
         <v>9999</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>135</v>
@@ -4354,12 +4354,12 @@
         <v>9999</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>138</v>
@@ -4371,12 +4371,12 @@
         <v>9999</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="171" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B171" s="5" t="s">
         <v>137</v>
@@ -4388,12 +4388,12 @@
         <v>9999</v>
       </c>
       <c r="E171" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>136</v>
@@ -4405,12 +4405,12 @@
         <v>9999</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>145</v>
@@ -4422,12 +4422,12 @@
         <v>9999</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="174" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B174" s="5" t="s">
         <v>144</v>
@@ -4439,12 +4439,12 @@
         <v>9999</v>
       </c>
       <c r="E174" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>146</v>
@@ -4456,15 +4456,15 @@
         <v>9999</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C176" s="2">
         <v>2005</v>
@@ -4473,12 +4473,12 @@
         <v>9999</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>148</v>
@@ -4490,12 +4490,12 @@
         <v>9999</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>147</v>
@@ -4507,15 +4507,15 @@
         <v>9999</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C179" s="2">
         <v>2006</v>
@@ -4524,12 +4524,12 @@
         <v>9999</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>149</v>
@@ -4541,15 +4541,15 @@
         <v>9999</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>348</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>349</v>
       </c>
       <c r="C181" s="2">
         <v>2007</v>
@@ -4558,12 +4558,12 @@
         <v>9999</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>151</v>
@@ -4575,12 +4575,12 @@
         <v>9999</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="183" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B183" s="5" t="s">
         <v>150</v>
@@ -4592,12 +4592,12 @@
         <v>9999</v>
       </c>
       <c r="E183" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>152</v>
@@ -4609,12 +4609,12 @@
         <v>9999</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>172</v>
@@ -4626,12 +4626,12 @@
         <v>9999</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>153</v>
@@ -4643,12 +4643,12 @@
         <v>9999</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="187" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B187" s="5" t="s">
         <v>154</v>
@@ -4660,12 +4660,12 @@
         <v>9999</v>
       </c>
       <c r="E187" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>155</v>
@@ -4677,12 +4677,12 @@
         <v>9999</v>
       </c>
       <c r="E188" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>156</v>
@@ -4694,12 +4694,12 @@
         <v>9999</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>157</v>
@@ -4711,12 +4711,12 @@
         <v>9999</v>
       </c>
       <c r="E190" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>158</v>
@@ -4728,12 +4728,12 @@
         <v>9999</v>
       </c>
       <c r="E191" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="192" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B192" s="5" t="s">
         <v>159</v>
@@ -4745,12 +4745,12 @@
         <v>9999</v>
       </c>
       <c r="E192" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>160</v>
@@ -4762,12 +4762,12 @@
         <v>9999</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>162</v>
@@ -4779,12 +4779,12 @@
         <v>9999</v>
       </c>
       <c r="E194" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>161</v>
@@ -4796,12 +4796,12 @@
         <v>9999</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="196" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B196" s="5" t="s">
         <v>163</v>
@@ -4813,12 +4813,12 @@
         <v>9999</v>
       </c>
       <c r="E196" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="197" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B197" s="5" t="s">
         <v>164</v>
@@ -4830,15 +4830,15 @@
         <v>9999</v>
       </c>
       <c r="E197" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="198" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C198" s="4">
         <v>2018</v>
@@ -4847,12 +4847,12 @@
         <v>9999</v>
       </c>
       <c r="E198" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>166</v>
@@ -4864,12 +4864,12 @@
         <v>9999</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>165</v>
@@ -4881,12 +4881,12 @@
         <v>9999</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>167</v>
@@ -4898,12 +4898,12 @@
         <v>9999</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>168</v>
@@ -4915,7 +4915,7 @@
         <v>9999</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reflects results of videoconference with Ken on 12/29/2020.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\prototype-historical-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFBBDD8-06C6-4642-845D-95B4B8E5E4D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{590C20E0-6708-4859-BAFC-9ED23CFE1496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{48B35B47-D791-4DB0-8E3F-11AF1DC17D23}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="feature_timeline" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="369">
   <si>
     <t>Middlesex Turnpike, opened 1811</t>
   </si>
@@ -375,15 +375,9 @@
     <t>Orange_Line-1908-1987</t>
   </si>
   <si>
-    <t>Red_LIne-1912</t>
-  </si>
-  <si>
     <t>Green_Line-1914</t>
   </si>
   <si>
-    <t>Red_LIne-1915</t>
-  </si>
-  <si>
     <t>Blue_Line-Bowdoin-1916</t>
   </si>
   <si>
@@ -507,15 +501,6 @@
     <t>Orange_Line-1987</t>
   </si>
   <si>
-    <t>Red_LIne-1985</t>
-  </si>
-  <si>
-    <t>Red_LIne-1984</t>
-  </si>
-  <si>
-    <t>Red_LIne-1980</t>
-  </si>
-  <si>
     <t>Orange_Line-1975</t>
   </si>
   <si>
@@ -525,9 +510,6 @@
     <t>I93-Tobin-128-1973</t>
   </si>
   <si>
-    <t>Red_LIne-1971</t>
-  </si>
-  <si>
     <t>I495-complete-1969</t>
   </si>
   <si>
@@ -633,9 +615,6 @@
     <t>Orange Line (Sullivan–Oak Grove)</t>
   </si>
   <si>
-    <t>Route-3-Norwell-Boston-1957</t>
-  </si>
-  <si>
     <t>Salem-Turnpike-1803-1868</t>
   </si>
   <si>
@@ -663,9 +642,6 @@
     <t>Worcester Turnpike (Route 9)</t>
   </si>
   <si>
-    <t>Union Turnpike (Route 2 west of concord)</t>
-  </si>
-  <si>
     <t>Cambridge-Concord Turnpike (Route 2 east of Concord), made public highway</t>
   </si>
   <si>
@@ -699,9 +675,6 @@
     <t>Interstate 90 (Worcester–I-495–Route 128)</t>
   </si>
   <si>
-    <t>I-93_SE_Expressway_Route3_Route24_I-95</t>
-  </si>
-  <si>
     <t>Interstate 93 (SE Expressway–Route 3–Route 24–I-95)</t>
   </si>
   <si>
@@ -726,108 +699,48 @@
     <t>Route 2 (Route 128–Alewife)</t>
   </si>
   <si>
-    <t>Framingham-commuter rail-1834</t>
-  </si>
-  <si>
     <t>Worcester commuter rail line (Boston–Framingham)</t>
   </si>
   <si>
-    <t>Providence-commuter rail-1834</t>
-  </si>
-  <si>
     <t>Providence commuter rail Line (Providence-Boston)</t>
   </si>
   <si>
-    <t>Lowell-commuter rail-1835</t>
-  </si>
-  <si>
     <t>Lowell commuter rail line (Lowell–Boston)</t>
   </si>
   <si>
-    <t>Haverhill-commuter rail-1837</t>
-  </si>
-  <si>
     <t>Haverhill commuter rail line (Wilmington–Bradford)</t>
   </si>
   <si>
-    <t>Newburyport-commuter rail-1838</t>
-  </si>
-  <si>
     <t>Newburyport commuter rail line (East Boston–Salem)</t>
   </si>
   <si>
-    <t>Newburyport-commuter rail-1839</t>
-  </si>
-  <si>
-    <t>Newburyport commuter rail line (Salem–Newburyport)</t>
-  </si>
-  <si>
-    <t>Fitchburg-commuter rail-1843</t>
-  </si>
-  <si>
-    <t>Fitchburg-commuter rail-1844</t>
-  </si>
-  <si>
     <t>Fitchburg commuter rail line (Waltham–Concord)</t>
   </si>
   <si>
-    <t>Fitchburg-commuter rail-1845</t>
-  </si>
-  <si>
     <t>Fitchburg commuter rail line (Concord–Fitchburg)</t>
   </si>
   <si>
-    <t>Rockport-commuter rail-1847</t>
-  </si>
-  <si>
     <t>Rockport commuter rail line (Beverly Depot–Gloucester)</t>
   </si>
   <si>
-    <t>Franklin-commuter rail-1849</t>
-  </si>
-  <si>
     <t>Franklin commuter rail line (Dedham–Franklin)</t>
   </si>
   <si>
-    <t>Needham-commuter rail-1850</t>
-  </si>
-  <si>
     <t>Needham commuter rail line (Forest Hills–West Roxbury)</t>
   </si>
   <si>
-    <t>Rockport-commuter rail-1861</t>
-  </si>
-  <si>
     <t>Rockport commuter rail line (Gloucester–Rockport)</t>
   </si>
   <si>
-    <t>Mcommuter railT-1875-1979</t>
-  </si>
-  <si>
-    <t>Stoughton-commuter rail-1888</t>
-  </si>
-  <si>
     <t>Stoughton commuter rail Line</t>
   </si>
   <si>
-    <t>Needham-commuter rail-1906</t>
-  </si>
-  <si>
     <t>Needham commuter rail line (West Roxbury–Needham Junction)</t>
   </si>
   <si>
-    <t>Needham-commuter rail-1907</t>
-  </si>
-  <si>
-    <t>Fairmount-commuter rail-1979</t>
-  </si>
-  <si>
     <t>Fairmount commuter rail line</t>
   </si>
   <si>
-    <t>Worcester-commuter rail-1994</t>
-  </si>
-  <si>
     <t>Worcester commuter rail line (Framingham–Worcester)</t>
   </si>
   <si>
@@ -837,21 +750,12 @@
     <t>Old Colony commuter rail line (Middleborough/Lakeville)</t>
   </si>
   <si>
-    <t>Newburyport-commuter rail-1999</t>
-  </si>
-  <si>
     <t>Newburyport commuter rail line (Ipswich–Newburyport)</t>
   </si>
   <si>
-    <t>Greenbush-commuter rail-2007</t>
-  </si>
-  <si>
     <t>Fitchburg commuter rail line (Fitchburg–Wachusett)</t>
   </si>
   <si>
-    <t>Mcommuter railT-2019</t>
-  </si>
-  <si>
     <t>Woburn_Branch_railroad-1844-1961</t>
   </si>
   <si>
@@ -861,9 +765,6 @@
     <t>Lowell-Nashua_railroad-1844-1966</t>
   </si>
   <si>
-    <t>Old_Colony_railroad-1845-1959</t>
-  </si>
-  <si>
     <t>Lowell-Lawrence_railroad-1846-1936</t>
   </si>
   <si>
@@ -1020,24 +921,6 @@
     <t>Eastern railroad (Marblehead)</t>
   </si>
   <si>
-    <t>Pierailroade_Lallement_Bike_Path-1987</t>
-  </si>
-  <si>
-    <t>Pierailroade Lallement Bike Path (Boston)</t>
-  </si>
-  <si>
-    <t>Narailroadow-Gauge-Trail-1992</t>
-  </si>
-  <si>
-    <t>Narailroadow Gauge Rail Trail (Bedford)</t>
-  </si>
-  <si>
-    <t>Old_Colony_railroad-1997</t>
-  </si>
-  <si>
-    <t>Old_Colony_railroad-1998</t>
-  </si>
-  <si>
     <t>Fitchburg commuter rail line (North Station–Waltham)</t>
   </si>
   <si>
@@ -1126,6 +1009,129 @@
   </si>
   <si>
     <t>Massachusetts Department of Public Works (DPW)</t>
+  </si>
+  <si>
+    <t>Framingham-CR-1834</t>
+  </si>
+  <si>
+    <t>Lowell-CR-1835</t>
+  </si>
+  <si>
+    <t>Haverhill-CR-1837</t>
+  </si>
+  <si>
+    <t>Newburyport-CR-1838</t>
+  </si>
+  <si>
+    <t>Newburyport-CR-1839</t>
+  </si>
+  <si>
+    <t>Fitchburg-CR-1843</t>
+  </si>
+  <si>
+    <t>Fitchburg-CR-1844</t>
+  </si>
+  <si>
+    <t>Fitchburg-CR-1845</t>
+  </si>
+  <si>
+    <t>Rockport-CR-1847</t>
+  </si>
+  <si>
+    <t>Franklin-CR-1849</t>
+  </si>
+  <si>
+    <t>Needham-CR-1850</t>
+  </si>
+  <si>
+    <t>Rockport-CR-1861</t>
+  </si>
+  <si>
+    <t>MCRT-1875-1979</t>
+  </si>
+  <si>
+    <t>Stoughton-CR-1888</t>
+  </si>
+  <si>
+    <t>Needham-CR-1906</t>
+  </si>
+  <si>
+    <t>Needham-CR-1907</t>
+  </si>
+  <si>
+    <t>Fairmount-CR-1979</t>
+  </si>
+  <si>
+    <t>Worcester-CR-1994</t>
+  </si>
+  <si>
+    <t>Newburyport-CR-1999</t>
+  </si>
+  <si>
+    <t>Greenbush-CR-2007</t>
+  </si>
+  <si>
+    <t>MCRT-2019</t>
+  </si>
+  <si>
+    <t>Red_Line-1912</t>
+  </si>
+  <si>
+    <t>Red_Line-1915</t>
+  </si>
+  <si>
+    <t>Red_Line-1971</t>
+  </si>
+  <si>
+    <t>Red_Line-1980</t>
+  </si>
+  <si>
+    <t>Red_Line-1984</t>
+  </si>
+  <si>
+    <t>Red_Line-1985</t>
+  </si>
+  <si>
+    <t>Pierre_Lallement_Bike_Path-1987</t>
+  </si>
+  <si>
+    <t>Pierre Lallement Bike Path (Boston)</t>
+  </si>
+  <si>
+    <t>Narrow-Gauge-Trail-1992</t>
+  </si>
+  <si>
+    <t>Narrow Gauge Rail Trail (Bedford)</t>
+  </si>
+  <si>
+    <t>Union Turnpike (Route 2 west of Concord)</t>
+  </si>
+  <si>
+    <t>Providence-CR-1834</t>
+  </si>
+  <si>
+    <t>I-93_SE_Expressway_Rt.3_Rt.24_I-95</t>
+  </si>
+  <si>
+    <t>Route-3-Boston-Norwell-1957</t>
+  </si>
+  <si>
+    <t>Newburyport-CR-1839-1976</t>
+  </si>
+  <si>
+    <t>Old_Colony_RR-1845-1959</t>
+  </si>
+  <si>
+    <t>Old_Colony_RR-1997</t>
+  </si>
+  <si>
+    <t>Old_Colony_RR-1998</t>
+  </si>
+  <si>
+    <t>Newburyport commuter rail line (Salem-Newburyport)</t>
+  </si>
+  <si>
+    <t>Newburyport commuter rail line (Ipswich-Newburyport)</t>
   </si>
 </sst>
 </file>
@@ -1502,15 +1508,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB246BE0-9101-4910-B137-94A0FD6048BC}">
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E203"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" style="5" customWidth="1"/>
     <col min="2" max="2" width="68.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="14" style="2" customWidth="1"/>
@@ -1519,10 +1525,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>207</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>83</v>
@@ -1538,7 +1544,7 @@
       <c r="A2" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0</v>
       </c>
       <c r="D2" s="4">
@@ -1552,7 +1558,7 @@
       <c r="A3" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
       <c r="D3" s="4">
@@ -1566,7 +1572,7 @@
       <c r="A4" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0</v>
       </c>
       <c r="D4" s="4">
@@ -1580,7 +1586,7 @@
       <c r="A5" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0</v>
       </c>
       <c r="D5" s="4">
@@ -1594,7 +1600,7 @@
       <c r="A6" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
       <c r="D6" s="4">
@@ -1608,7 +1614,7 @@
       <c r="A7" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0</v>
       </c>
       <c r="D7" s="4">
@@ -1622,7 +1628,7 @@
       <c r="A8" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0</v>
       </c>
       <c r="D8" s="4">
@@ -1636,7 +1642,7 @@
       <c r="A9" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0</v>
       </c>
       <c r="D9" s="4">
@@ -1650,7 +1656,7 @@
       <c r="A10" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0</v>
       </c>
       <c r="D10" s="4">
@@ -1676,10 +1682,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C12" s="2">
         <v>1803</v>
@@ -1696,7 +1702,7 @@
         <v>104</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C13" s="2">
         <v>1804</v>
@@ -1713,7 +1719,7 @@
         <v>105</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C14" s="2">
         <v>1805</v>
@@ -1730,7 +1736,7 @@
         <v>106</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>339</v>
+        <v>300</v>
       </c>
       <c r="C15" s="2">
         <v>1806</v>
@@ -1747,7 +1753,7 @@
         <v>107</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>340</v>
+        <v>301</v>
       </c>
       <c r="C16" s="2">
         <v>1807</v>
@@ -1764,7 +1770,7 @@
         <v>108</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C17" s="2">
         <v>1808</v>
@@ -1781,7 +1787,7 @@
         <v>109</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>212</v>
+        <v>359</v>
       </c>
       <c r="C18" s="2">
         <v>1809</v>
@@ -1812,7 +1818,7 @@
     </row>
     <row r="20" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>1</v>
@@ -1829,7 +1835,7 @@
     </row>
     <row r="21" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>2</v>
@@ -1846,10 +1852,10 @@
     </row>
     <row r="22" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>341</v>
+        <v>302</v>
       </c>
       <c r="C22" s="4">
         <v>1826</v>
@@ -1863,7 +1869,7 @@
     </row>
     <row r="23" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>3</v>
@@ -1880,10 +1886,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C24" s="4">
         <v>1829</v>
@@ -1897,10 +1903,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B25" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C25" s="4">
         <v>1830</v>
@@ -1914,10 +1920,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>233</v>
+        <v>328</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C26" s="2">
         <v>1834</v>
@@ -1931,10 +1937,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>235</v>
+        <v>360</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="C27" s="2">
         <v>1834</v>
@@ -1948,10 +1954,10 @@
     </row>
     <row r="28" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>237</v>
+        <v>329</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="C28" s="2">
         <v>1835</v>
@@ -1965,10 +1971,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>239</v>
+        <v>330</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C29" s="2">
         <v>1837</v>
@@ -1982,10 +1988,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C30" s="4">
         <v>1838</v>
@@ -1999,10 +2005,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>241</v>
+        <v>331</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="C31" s="2">
         <v>1838</v>
@@ -2016,33 +2022,30 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>243</v>
+        <v>332</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>244</v>
+        <v>367</v>
       </c>
       <c r="C32" s="2">
         <v>1839</v>
       </c>
-      <c r="D32" s="4">
-        <v>1976</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>89</v>
+      <c r="D32" s="2">
+        <v>9999</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>245</v>
+        <v>363</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>337</v>
+        <v>368</v>
       </c>
       <c r="C33" s="2">
-        <v>1843</v>
-      </c>
-      <c r="D33" s="2">
-        <v>9999</v>
+        <v>1839</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1976</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>89</v>
@@ -2050,152 +2053,152 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>275</v>
+        <v>333</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>276</v>
+        <v>298</v>
       </c>
       <c r="C34" s="2">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="D34" s="2">
-        <v>1961</v>
+        <v>9999</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>246</v>
+      <c r="A35" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C35" s="2">
         <v>1844</v>
       </c>
       <c r="D35" s="2">
-        <v>9999</v>
+        <v>1961</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>277</v>
+      <c r="A36" t="s">
+        <v>334</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>338</v>
+        <v>229</v>
       </c>
       <c r="C36" s="2">
         <v>1844</v>
       </c>
       <c r="D36" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1844</v>
+      </c>
+      <c r="D37" s="2">
         <v>1966</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>178</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C37" s="4">
+      <c r="E37" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>172</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38" s="4">
         <v>1845</v>
       </c>
-      <c r="D37" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1845</v>
-      </c>
-      <c r="D38" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>278</v>
+        <v>335</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>342</v>
+        <v>230</v>
       </c>
       <c r="C39" s="2">
         <v>1845</v>
       </c>
       <c r="D39" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1845</v>
+      </c>
+      <c r="D40" s="2">
         <v>1959</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="C40" s="4">
+      <c r="E40" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C41" s="4">
         <v>1846</v>
       </c>
-      <c r="D40" s="4">
+      <c r="D41" s="4">
         <v>1959</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C41" s="2">
-        <v>1846</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1936</v>
-      </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
       <c r="C42" s="2">
         <v>1846</v>
       </c>
       <c r="D42" s="2">
-        <v>1941</v>
+        <v>1936</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>89</v>
@@ -2203,16 +2206,16 @@
     </row>
     <row r="43" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>282</v>
+        <v>247</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="C43" s="2">
         <v>1846</v>
       </c>
       <c r="D43" s="2">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>89</v>
@@ -2220,16 +2223,16 @@
     </row>
     <row r="44" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>284</v>
+        <v>249</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>285</v>
+        <v>250</v>
       </c>
       <c r="C44" s="2">
         <v>1846</v>
       </c>
       <c r="D44" s="2">
-        <v>1981</v>
+        <v>1943</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>89</v>
@@ -2237,33 +2240,33 @@
     </row>
     <row r="45" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C45" s="2">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="D45" s="2">
-        <v>9999</v>
+        <v>1981</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>286</v>
+        <v>336</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>287</v>
+        <v>231</v>
       </c>
       <c r="C46" s="2">
         <v>1847</v>
       </c>
       <c r="D46" s="2">
-        <v>1863</v>
+        <v>9999</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>89</v>
@@ -2271,16 +2274,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>288</v>
+        <v>253</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>289</v>
+        <v>254</v>
       </c>
       <c r="C47" s="2">
         <v>1847</v>
       </c>
       <c r="D47" s="2">
-        <v>1960</v>
+        <v>1863</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>89</v>
@@ -2288,10 +2291,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>290</v>
+        <v>255</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="C48" s="2">
         <v>1847</v>
@@ -2304,17 +2307,17 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>292</v>
+      <c r="A49" s="5" t="s">
+        <v>257</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>293</v>
+        <v>258</v>
       </c>
       <c r="C49" s="2">
         <v>1847</v>
       </c>
       <c r="D49" s="2">
-        <v>1980</v>
+        <v>1960</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>89</v>
@@ -2322,10 +2325,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>294</v>
+        <v>259</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>295</v>
+        <v>260</v>
       </c>
       <c r="C50" s="2">
         <v>1847</v>
@@ -2339,33 +2342,33 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>296</v>
+        <v>261</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>297</v>
+        <v>262</v>
       </c>
       <c r="C51" s="2">
         <v>1847</v>
       </c>
       <c r="D51" s="2">
+        <v>1980</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>263</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C52" s="2">
+        <v>1847</v>
+      </c>
+      <c r="D52" s="2">
         <v>1985</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C52" s="2">
-        <v>1848</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1861</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>89</v>
@@ -2373,16 +2376,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="C53" s="2">
         <v>1848</v>
       </c>
       <c r="D53" s="2">
-        <v>1972</v>
+        <v>1861</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>89</v>
@@ -2390,16 +2393,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>302</v>
+        <v>267</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>303</v>
+        <v>268</v>
       </c>
       <c r="C54" s="2">
         <v>1848</v>
       </c>
       <c r="D54" s="2">
-        <v>1981</v>
+        <v>1972</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>89</v>
@@ -2407,16 +2410,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>304</v>
+        <v>269</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>305</v>
+        <v>270</v>
       </c>
       <c r="C55" s="2">
         <v>1848</v>
       </c>
       <c r="D55" s="2">
-        <v>2011</v>
+        <v>1981</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>89</v>
@@ -2424,16 +2427,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>253</v>
+        <v>272</v>
       </c>
       <c r="C56" s="2">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="D56" s="2">
-        <v>9999</v>
+        <v>2011</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>89</v>
@@ -2441,50 +2444,50 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>306</v>
+        <v>337</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>307</v>
+        <v>232</v>
       </c>
       <c r="C57" s="2">
         <v>1849</v>
       </c>
       <c r="D57" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C58" s="2">
+        <v>1849</v>
+      </c>
+      <c r="D58" s="2">
         <v>1992</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="C58" s="2">
-        <v>1850</v>
-      </c>
-      <c r="D58" s="2">
-        <v>9999</v>
-      </c>
       <c r="E58" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>191</v>
+        <v>338</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>308</v>
+        <v>233</v>
       </c>
       <c r="C59" s="2">
         <v>1850</v>
       </c>
       <c r="D59" s="2">
-        <v>1980</v>
+        <v>9999</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>89</v>
@@ -2492,16 +2495,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>309</v>
+        <v>185</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>4</v>
+        <v>275</v>
       </c>
       <c r="C60" s="2">
         <v>1850</v>
       </c>
       <c r="D60" s="2">
-        <v>9999</v>
+        <v>1980</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>89</v>
@@ -2509,16 +2512,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>310</v>
+        <v>276</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>311</v>
+        <v>4</v>
       </c>
       <c r="C61" s="2">
         <v>1850</v>
       </c>
       <c r="D61" s="2">
-        <v>1993</v>
+        <v>9999</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>89</v>
@@ -2526,16 +2529,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>313</v>
+        <v>278</v>
       </c>
       <c r="C62" s="2">
         <v>1850</v>
       </c>
       <c r="D62" s="2">
-        <v>1987</v>
+        <v>1993</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>89</v>
@@ -2543,16 +2546,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>314</v>
+        <v>279</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>5</v>
+        <v>280</v>
       </c>
       <c r="C63" s="2">
-        <v>1853</v>
+        <v>1850</v>
       </c>
       <c r="D63" s="2">
-        <v>1927</v>
+        <v>1987</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>89</v>
@@ -2560,16 +2563,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>315</v>
+        <v>281</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>316</v>
+        <v>5</v>
       </c>
       <c r="C64" s="2">
         <v>1853</v>
       </c>
       <c r="D64" s="2">
-        <v>1958</v>
+        <v>1927</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>89</v>
@@ -2577,84 +2580,84 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>317</v>
+        <v>282</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>318</v>
+        <v>283</v>
       </c>
       <c r="C65" s="2">
+        <v>1853</v>
+      </c>
+      <c r="D65" s="2">
+        <v>1958</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C66" s="2">
         <v>1855</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D66" s="2">
         <v>1981</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="C66" s="4">
+      <c r="E66" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C67" s="4">
         <v>1856</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <v>1912</v>
       </c>
-      <c r="E66" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>179</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C67" s="4">
+      <c r="E67" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>173</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C68" s="4">
         <v>1857</v>
       </c>
-      <c r="D67" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C68" s="2">
-        <v>1861</v>
-      </c>
-      <c r="D68" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>89</v>
+      <c r="D68" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>192</v>
+        <v>339</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>319</v>
+        <v>234</v>
       </c>
       <c r="C69" s="2">
         <v>1861</v>
       </c>
       <c r="D69" s="2">
-        <v>1976</v>
+        <v>9999</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>89</v>
@@ -2662,101 +2665,101 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>320</v>
+        <v>186</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>321</v>
+        <v>286</v>
       </c>
       <c r="C70" s="2">
+        <v>1861</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1976</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C71" s="2">
         <v>1867</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D71" s="2">
         <v>1993</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>180</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C71" s="4">
+      <c r="E71" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>174</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C72" s="4">
         <v>1868</v>
       </c>
-      <c r="D71" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C72" s="2">
-        <v>1871</v>
-      </c>
-      <c r="D72" s="2">
-        <v>2001</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>89</v>
+      <c r="D72" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>324</v>
+        <v>289</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>325</v>
+        <v>290</v>
       </c>
       <c r="C73" s="2">
-        <v>1873</v>
+        <v>1871</v>
       </c>
       <c r="D73" s="2">
-        <v>1993</v>
+        <v>2001</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>199</v>
+        <v>291</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>6</v>
+        <v>292</v>
       </c>
       <c r="C74" s="2">
         <v>1873</v>
       </c>
       <c r="D74" s="2">
+        <v>1993</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" s="2">
+        <v>1873</v>
+      </c>
+      <c r="D75" s="2">
         <v>1924</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>326</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C75" s="2">
-        <v>1874</v>
-      </c>
-      <c r="D75" s="2">
-        <v>1920</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>89</v>
@@ -2764,16 +2767,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>258</v>
+        <v>293</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>328</v>
+        <v>294</v>
       </c>
       <c r="C76" s="2">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="D76" s="2">
-        <v>1979</v>
+        <v>1920</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>89</v>
@@ -2781,16 +2784,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>330</v>
+        <v>295</v>
       </c>
       <c r="C77" s="2">
-        <v>1886</v>
+        <v>1875</v>
       </c>
       <c r="D77" s="2">
-        <v>1961</v>
+        <v>1979</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>89</v>
@@ -2798,98 +2801,98 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>259</v>
+        <v>296</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>260</v>
+        <v>297</v>
       </c>
       <c r="C78" s="2">
+        <v>1886</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1961</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C79" s="2">
         <v>1888</v>
       </c>
-      <c r="D78" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B79" s="1" t="s">
+      <c r="D79" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C80" s="2">
         <v>1889</v>
       </c>
-      <c r="D79" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E79" s="2" t="s">
+      <c r="D80" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" s="2">
-        <v>1894</v>
-      </c>
-      <c r="D80" s="2">
-        <v>1919</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C81" s="2">
         <v>1894</v>
       </c>
       <c r="D81" s="2">
-        <v>9999</v>
+        <v>1919</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>193</v>
+        <v>118</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>346</v>
+        <v>9</v>
       </c>
       <c r="C82" s="2">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="D82" s="2">
         <v>9999</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>347</v>
+        <v>307</v>
       </c>
       <c r="C83" s="2">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="D83" s="2">
         <v>9999</v>
@@ -2900,81 +2903,81 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>120</v>
+        <v>184</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C84" s="2">
+        <v>1898</v>
+      </c>
+      <c r="D84" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C85" s="2">
         <v>1899</v>
       </c>
-      <c r="D84" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>111</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C85" s="2">
-        <v>1901</v>
-      </c>
       <c r="D85" s="2">
-        <v>1987</v>
+        <v>9999</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C86" s="2">
         <v>1901</v>
       </c>
       <c r="D86" s="2">
-        <v>1938</v>
+        <v>1987</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
-        <v>113</v>
+      <c r="A87" t="s">
+        <v>112</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C87" s="2">
         <v>1901</v>
       </c>
       <c r="D87" s="2">
-        <v>9999</v>
+        <v>1938</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>114</v>
+      <c r="A88" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C88" s="2">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="D88" s="2">
         <v>9999</v>
@@ -2984,14 +2987,14 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
-        <v>261</v>
+      <c r="A89" t="s">
+        <v>114</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>262</v>
+        <v>14</v>
       </c>
       <c r="C89" s="2">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="D89" s="2">
         <v>9999</v>
@@ -3002,13 +3005,13 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>263</v>
+        <v>342</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>351</v>
+        <v>236</v>
       </c>
       <c r="C90" s="2">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="D90" s="2">
         <v>9999</v>
@@ -3018,17 +3021,17 @@
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>115</v>
+      <c r="A91" s="5" t="s">
+        <v>343</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
       <c r="C91" s="2">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="D91" s="2">
-        <v>1987</v>
+        <v>9999</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>88</v>
@@ -3036,16 +3039,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>348</v>
+        <v>15</v>
       </c>
       <c r="C92" s="2">
-        <v>1912</v>
+        <v>1908</v>
       </c>
       <c r="D92" s="2">
-        <v>9999</v>
+        <v>1987</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>88</v>
@@ -3053,10 +3056,10 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>349</v>
+        <v>309</v>
       </c>
       <c r="C93" s="2">
         <v>1912</v>
@@ -3069,14 +3072,14 @@
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>117</v>
+      <c r="A94" t="s">
+        <v>349</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>16</v>
+        <v>310</v>
       </c>
       <c r="C94" s="2">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="D94" s="2">
         <v>9999</v>
@@ -3087,13 +3090,13 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>350</v>
+        <v>16</v>
       </c>
       <c r="C95" s="2">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="D95" s="2">
         <v>9999</v>
@@ -3104,13 +3107,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>119</v>
+        <v>350</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>17</v>
+        <v>311</v>
       </c>
       <c r="C96" s="2">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="D96" s="2">
         <v>9999</v>
@@ -3121,13 +3124,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>194</v>
+        <v>117</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>352</v>
+        <v>17</v>
       </c>
       <c r="C97" s="2">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="D97" s="2">
         <v>9999</v>
@@ -3138,13 +3141,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="C98" s="2">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="D98" s="2">
         <v>9999</v>
@@ -3155,98 +3158,98 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>366</v>
+        <v>314</v>
       </c>
       <c r="C99" s="2">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="D99" s="2">
-        <v>2009</v>
+        <v>9999</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>121</v>
+      <c r="A100" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>18</v>
+        <v>327</v>
       </c>
       <c r="C100" s="2">
         <v>1919</v>
       </c>
       <c r="D100" s="2">
+        <v>2009</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>119</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" s="2">
+        <v>1919</v>
+      </c>
+      <c r="D101" s="2">
         <v>1975</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C101" s="2">
-        <v>1922</v>
-      </c>
-      <c r="D101" s="2">
-        <v>9999</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>122</v>
+      <c r="A102" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C102" s="2">
+        <v>1922</v>
+      </c>
+      <c r="D102" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>120</v>
+      </c>
+      <c r="B103" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C102" s="2">
+      <c r="C103" s="2">
         <v>1923</v>
       </c>
-      <c r="D102" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E102" s="2" t="s">
+      <c r="D103" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C103" s="2">
-        <v>1927</v>
-      </c>
-      <c r="D103" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C104" s="2">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="D104" s="2">
         <v>9999</v>
@@ -3257,13 +3260,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C105" s="2">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="D105" s="2">
         <v>9999</v>
@@ -3274,61 +3277,61 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>123</v>
+        <v>197</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C106" s="2">
-        <v>1934</v>
+        <v>1929</v>
       </c>
       <c r="D106" s="2">
         <v>9999</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>354</v>
+        <v>24</v>
       </c>
       <c r="C107" s="2">
+        <v>1934</v>
+      </c>
+      <c r="D107" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C108" s="2">
         <v>1936</v>
       </c>
-      <c r="D107" s="2">
+      <c r="D108" s="2">
         <v>1963</v>
       </c>
-      <c r="E107" s="2" t="s">
+      <c r="E108" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>125</v>
-      </c>
-      <c r="B108" s="1" t="s">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>123</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C108" s="2">
-        <v>1941</v>
-      </c>
-      <c r="D108" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C109" s="2">
         <v>1941</v>
@@ -3337,69 +3340,69 @@
         <v>9999</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C110" s="2">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="D110" s="2">
         <v>9999</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>365</v>
+        <v>27</v>
       </c>
       <c r="C111" s="2">
-        <v>1947</v>
+        <v>1943</v>
       </c>
       <c r="D111" s="2">
-        <v>1964</v>
+        <v>9999</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C112" s="2">
+        <v>1947</v>
+      </c>
+      <c r="D112" s="2">
+        <v>1964</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C112" s="2">
+      <c r="C113" s="2">
         <v>1950</v>
-      </c>
-      <c r="D112" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>127</v>
-      </c>
-      <c r="B113" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C113" s="2">
-        <v>1951</v>
       </c>
       <c r="D113" s="2">
         <v>9999</v>
@@ -3410,13 +3413,13 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
       <c r="C114" s="2">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="D114" s="2">
         <v>9999</v>
@@ -3426,17 +3429,17 @@
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
-        <v>120</v>
+      <c r="A115" t="s">
+        <v>175</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>30</v>
+        <v>176</v>
       </c>
       <c r="C115" s="2">
         <v>1952</v>
       </c>
       <c r="D115" s="2">
-        <v>2009</v>
+        <v>9999</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>86</v>
@@ -3444,44 +3447,44 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C116" s="2">
         <v>1952</v>
       </c>
       <c r="D116" s="2">
-        <v>9999</v>
+        <v>2009</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C117" s="2">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="D117" s="2">
         <v>9999</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>220</v>
+        <v>32</v>
       </c>
       <c r="C118" s="2">
         <v>1954</v>
@@ -3498,7 +3501,7 @@
         <v>129</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>31</v>
+        <v>212</v>
       </c>
       <c r="C119" s="2">
         <v>1954</v>
@@ -3507,72 +3510,72 @@
         <v>9999</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>221</v>
+        <v>31</v>
       </c>
       <c r="C120" s="2">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="D120" s="2">
         <v>9999</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>33</v>
+        <v>213</v>
       </c>
       <c r="C121" s="2">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="D121" s="2">
         <v>9999</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="C122" s="2">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="D122" s="2">
-        <v>2016</v>
+        <v>9999</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>202</v>
+        <v>118</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>222</v>
+        <v>82</v>
       </c>
       <c r="C123" s="2">
         <v>1957</v>
       </c>
       <c r="D123" s="2">
-        <v>9999</v>
+        <v>2016</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>86</v>
@@ -3580,10 +3583,10 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>172</v>
+        <v>362</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C124" s="2">
         <v>1957</v>
@@ -3597,67 +3600,67 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="B125" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C125" s="2">
+        <v>1957</v>
+      </c>
+      <c r="D125" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B126" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C125" s="2">
+      <c r="C126" s="2">
         <v>1958</v>
       </c>
-      <c r="D125" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C126" s="4">
+      <c r="D126" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C127" s="4">
         <v>1958</v>
       </c>
-      <c r="D126" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E126" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C127" s="2">
-        <v>1958</v>
-      </c>
-      <c r="D127" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E127" s="2" t="s">
+      <c r="D127" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E127" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>81</v>
+        <v>217</v>
       </c>
       <c r="C128" s="2">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="D128" s="2">
-        <v>2004</v>
+        <v>9999</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>86</v>
@@ -3665,16 +3668,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C129" s="2">
         <v>1959</v>
       </c>
       <c r="D129" s="2">
-        <v>9999</v>
+        <v>2004</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>86</v>
@@ -3682,10 +3685,10 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C130" s="2">
         <v>1959</v>
@@ -3694,49 +3697,49 @@
         <v>9999</v>
       </c>
       <c r="E130" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C131" s="2">
+        <v>1959</v>
+      </c>
+      <c r="D131" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E131" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="131" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B131" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C131" s="4">
+    <row r="132" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C132" s="4">
         <v>1961</v>
       </c>
-      <c r="D131" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E131" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B132" s="1" t="s">
+      <c r="D132" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C132" s="2">
-        <v>1962</v>
-      </c>
-      <c r="D132" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>170</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="C133" s="2">
         <v>1962</v>
@@ -3749,11 +3752,11 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
-        <v>136</v>
+      <c r="A134" t="s">
+        <v>164</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>37</v>
+        <v>219</v>
       </c>
       <c r="C134" s="2">
         <v>1962</v>
@@ -3767,31 +3770,31 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>196</v>
+        <v>134</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>229</v>
+        <v>37</v>
       </c>
       <c r="C135" s="2">
+        <v>1962</v>
+      </c>
+      <c r="D135" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C136" s="2">
         <v>1963</v>
       </c>
-      <c r="D135" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>184</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C136" s="2">
-        <v>1964</v>
-      </c>
       <c r="D136" s="2">
         <v>9999</v>
       </c>
@@ -3800,11 +3803,11 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="5" t="s">
-        <v>185</v>
+      <c r="A137" t="s">
+        <v>178</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>38</v>
+        <v>221</v>
       </c>
       <c r="C137" s="2">
         <v>1964</v>
@@ -3818,10 +3821,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>120</v>
+        <v>179</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>363</v>
+        <v>38</v>
       </c>
       <c r="C138" s="2">
         <v>1964</v>
@@ -3830,29 +3833,32 @@
         <v>9999</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>186</v>
+        <v>118</v>
       </c>
       <c r="B139" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C139" s="2">
+        <v>1964</v>
+      </c>
+      <c r="D139" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B140" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C139" s="2">
-        <v>1965</v>
-      </c>
-      <c r="D139" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E139" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B140" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="C140" s="2">
         <v>1965</v>
@@ -3865,11 +3871,11 @@
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>169</v>
+      <c r="A141" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C141" s="2">
         <v>1965</v>
@@ -3883,13 +3889,13 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>40</v>
+        <v>223</v>
       </c>
       <c r="C142" s="2">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="D142" s="2">
         <v>9999</v>
@@ -3900,129 +3906,129 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B143" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C143" s="2">
+        <v>1966</v>
+      </c>
+      <c r="D143" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>161</v>
+      </c>
+      <c r="B144" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C143" s="2">
+      <c r="C144" s="2">
         <v>1969</v>
       </c>
-      <c r="D143" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B144" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C144" s="4">
+      <c r="D144" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C145" s="4">
         <v>1970</v>
       </c>
-      <c r="D144" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E144" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B145" s="1" t="s">
+      <c r="D145" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B146" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C145" s="2">
+      <c r="C146" s="2">
         <v>1971</v>
       </c>
-      <c r="D145" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E145" s="2" t="s">
+      <c r="D146" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E146" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>165</v>
-      </c>
-      <c r="B146" s="1" t="s">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>160</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C146" s="2">
+      <c r="C147" s="2">
         <v>1973</v>
       </c>
-      <c r="D146" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E146" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B147" s="1" t="s">
+      <c r="D147" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C147" s="2">
+      <c r="C148" s="2">
         <v>1974</v>
       </c>
-      <c r="D147" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E147" s="2" t="s">
+      <c r="D148" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E148" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>164</v>
-      </c>
-      <c r="B148" s="1" t="s">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>159</v>
+      </c>
+      <c r="B149" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C148" s="2">
+      <c r="C149" s="2">
         <v>1975</v>
       </c>
-      <c r="D148" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E148" s="2" t="s">
+      <c r="D149" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E149" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="149" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B149" s="5" t="s">
+    <row r="150" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B150" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="C149" s="4">
-        <v>1975</v>
-      </c>
-      <c r="D149" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E149" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B150" s="5" t="s">
-        <v>361</v>
       </c>
       <c r="C150" s="4">
         <v>1975</v>
@@ -4031,15 +4037,15 @@
         <v>9999</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>201</v>
+        <v>322</v>
       </c>
       <c r="C151" s="4">
         <v>1975</v>
@@ -4051,66 +4057,66 @@
         <v>88</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="C152" s="2">
+        <v>158</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C152" s="4">
+        <v>1975</v>
+      </c>
+      <c r="D152" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C153" s="2">
         <v>1979</v>
       </c>
-      <c r="D152" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E152" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B153" s="5" t="s">
-        <v>362</v>
-      </c>
-      <c r="C153" s="4">
+      <c r="D153" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C154" s="4">
         <v>1980</v>
       </c>
-      <c r="D153" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E153" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C154" s="2">
-        <v>1984</v>
-      </c>
-      <c r="D154" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E154" s="2" t="s">
+      <c r="D154" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E154" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>160</v>
+        <v>353</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C155" s="2">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="D155" s="2">
         <v>9999</v>
@@ -4121,27 +4127,27 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>332</v>
+        <v>46</v>
       </c>
       <c r="C156" s="2">
-        <v>1987</v>
+        <v>1985</v>
       </c>
       <c r="D156" s="2">
         <v>9999</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>159</v>
+        <v>355</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>47</v>
+        <v>356</v>
       </c>
       <c r="C157" s="2">
         <v>1987</v>
@@ -4150,32 +4156,32 @@
         <v>9999</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C158" s="2">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="D158" s="2">
         <v>9999</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>333</v>
+        <v>156</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>334</v>
+        <v>58</v>
       </c>
       <c r="C159" s="2">
         <v>1992</v>
@@ -4187,97 +4193,97 @@
         <v>92</v>
       </c>
     </row>
-    <row r="160" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B160" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="C160" s="4">
-        <v>1993</v>
-      </c>
-      <c r="D160" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E160" s="4" t="s">
-        <v>86</v>
+        <v>357</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C160" s="2">
+        <v>1992</v>
+      </c>
+      <c r="D160" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="161" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B161" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C161" s="4">
+        <v>1993</v>
+      </c>
+      <c r="D161" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B162" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C161" s="4">
+      <c r="C162" s="4">
         <v>1994</v>
       </c>
-      <c r="D161" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E161" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>266</v>
-      </c>
-      <c r="B162" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C162" s="2">
+      <c r="D162" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E162" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>345</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C163" s="2">
         <v>1994</v>
       </c>
-      <c r="D162" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B163" s="5" t="s">
+      <c r="D163" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B164" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C163" s="4">
+      <c r="C164" s="4">
         <v>1995</v>
       </c>
-      <c r="D163" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E163" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B164" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C164" s="2">
-        <v>1995</v>
-      </c>
-      <c r="D164" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E164" s="2" t="s">
+      <c r="D164" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E164" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C165" s="2">
         <v>1995</v>
@@ -4286,69 +4292,69 @@
         <v>9999</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>335</v>
+        <v>118</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>268</v>
+        <v>49</v>
       </c>
       <c r="C166" s="2">
+        <v>1995</v>
+      </c>
+      <c r="D166" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C167" s="2">
         <v>1997</v>
       </c>
-      <c r="D166" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B167" s="5" t="s">
+      <c r="D167" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B168" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C167" s="4">
+      <c r="C168" s="4">
         <v>1998</v>
       </c>
-      <c r="D167" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E167" s="4" t="s">
+      <c r="D168" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E168" s="4" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>336</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C168" s="2">
-        <v>1998</v>
-      </c>
-      <c r="D168" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E168" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>270</v>
+        <v>366</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>271</v>
+        <v>240</v>
       </c>
       <c r="C169" s="2">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="D169" s="2">
         <v>9999</v>
@@ -4359,129 +4365,129 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>156</v>
+        <v>346</v>
       </c>
       <c r="B170" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C170" s="2">
+        <v>1999</v>
+      </c>
+      <c r="D170" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>154</v>
+      </c>
+      <c r="B171" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C170" s="2">
+      <c r="C171" s="2">
         <v>2002</v>
       </c>
-      <c r="D170" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E170" s="2" t="s">
+      <c r="D171" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E171" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="171" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B171" s="5" t="s">
+    <row r="172" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B172" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C171" s="4">
+      <c r="C172" s="4">
         <v>2002</v>
       </c>
-      <c r="D171" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E171" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>155</v>
-      </c>
-      <c r="B172" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C172" s="2">
-        <v>2002</v>
-      </c>
-      <c r="D172" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E172" s="2" t="s">
-        <v>88</v>
+      <c r="D172" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E172" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B173" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C173" s="2">
+        <v>2002</v>
+      </c>
+      <c r="D173" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>152</v>
+      </c>
+      <c r="B174" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C173" s="2">
+      <c r="C174" s="2">
         <v>2003</v>
       </c>
-      <c r="D173" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E173" s="2" t="s">
+      <c r="D174" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E174" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="174" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B174" s="5" t="s">
+    <row r="175" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B175" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C174" s="4">
+      <c r="C175" s="4">
         <v>2003</v>
       </c>
-      <c r="D174" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E174" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>153</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C175" s="2">
-        <v>2003</v>
-      </c>
-      <c r="D175" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E175" s="2" t="s">
-        <v>88</v>
+      <c r="D175" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E175" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>356</v>
+        <v>61</v>
       </c>
       <c r="C176" s="2">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="D176" s="2">
         <v>9999</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="5" t="s">
-        <v>120</v>
+      <c r="A177" t="s">
+        <v>150</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>63</v>
+        <v>317</v>
       </c>
       <c r="C177" s="2">
         <v>2005</v>
@@ -4490,15 +4496,15 @@
         <v>9999</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C178" s="2">
         <v>2005</v>
@@ -4507,35 +4513,35 @@
         <v>9999</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>151</v>
+      <c r="A179" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>357</v>
+        <v>62</v>
       </c>
       <c r="C179" s="2">
+        <v>2005</v>
+      </c>
+      <c r="D179" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>149</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C180" s="2">
         <v>2006</v>
-      </c>
-      <c r="D179" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E179" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C180" s="2">
-        <v>2007</v>
       </c>
       <c r="D180" s="2">
         <v>9999</v>
@@ -4546,10 +4552,10 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>272</v>
+        <v>148</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>197</v>
+        <v>64</v>
       </c>
       <c r="C181" s="2">
         <v>2007</v>
@@ -4558,66 +4564,66 @@
         <v>9999</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>144</v>
+      <c r="A182" s="5" t="s">
+        <v>347</v>
       </c>
       <c r="B182" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C182" s="2">
+        <v>2007</v>
+      </c>
+      <c r="D182" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>142</v>
+      </c>
+      <c r="B183" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C182" s="2">
+      <c r="C183" s="2">
         <v>2008</v>
       </c>
-      <c r="D182" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E182" s="2" t="s">
+      <c r="D183" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E183" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="183" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B183" s="5" t="s">
+    <row r="184" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B184" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C183" s="4">
+      <c r="C184" s="4">
         <v>2008</v>
       </c>
-      <c r="D183" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E183" s="4" t="s">
+      <c r="D184" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E184" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>141</v>
-      </c>
-      <c r="B184" s="1" t="s">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>139</v>
+      </c>
+      <c r="B185" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C184" s="2">
-        <v>2009</v>
-      </c>
-      <c r="D184" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E184" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B185" s="1" t="s">
-        <v>358</v>
       </c>
       <c r="C185" s="2">
         <v>2009</v>
@@ -4626,15 +4632,15 @@
         <v>9999</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>142</v>
+      <c r="A186" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>68</v>
+        <v>319</v>
       </c>
       <c r="C186" s="2">
         <v>2009</v>
@@ -4643,49 +4649,49 @@
         <v>9999</v>
       </c>
       <c r="E186" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>140</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C187" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D187" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E187" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="187" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B187" s="5" t="s">
+    <row r="188" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B188" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C187" s="4">
+      <c r="C188" s="4">
         <v>2010</v>
       </c>
-      <c r="D187" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E187" s="4" t="s">
+      <c r="D188" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E188" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>143</v>
-      </c>
-      <c r="B188" s="1" t="s">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>141</v>
+      </c>
+      <c r="B189" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C188" s="2">
-        <v>2012</v>
-      </c>
-      <c r="D188" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E188" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B189" s="1" t="s">
-        <v>359</v>
       </c>
       <c r="C189" s="2">
         <v>2012</v>
@@ -4698,14 +4704,14 @@
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>140</v>
+      <c r="A190" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>71</v>
+        <v>320</v>
       </c>
       <c r="C190" s="2">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="D190" s="2">
         <v>9999</v>
@@ -4716,13 +4722,13 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C191" s="2">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D191" s="2">
         <v>9999</v>
@@ -4731,46 +4737,46 @@
         <v>92</v>
       </c>
     </row>
-    <row r="192" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B192" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="C192" s="4">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>143</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C192" s="2">
         <v>2014</v>
       </c>
-      <c r="D192" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E192" s="4" t="s">
+      <c r="D192" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C193" s="4">
+        <v>2014</v>
+      </c>
+      <c r="D193" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E193" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B193" s="1" t="s">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B194" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C193" s="2">
-        <v>2015</v>
-      </c>
-      <c r="D193" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E193" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" t="s">
-        <v>147</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C194" s="2">
         <v>2015</v>
@@ -4784,10 +4790,10 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C195" s="2">
         <v>2015</v>
@@ -4799,80 +4805,80 @@
         <v>92</v>
       </c>
     </row>
-    <row r="196" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B196" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="C196" s="4">
-        <v>2016</v>
-      </c>
-      <c r="D196" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E196" s="4" t="s">
-        <v>89</v>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>146</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C196" s="2">
+        <v>2015</v>
+      </c>
+      <c r="D196" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E196" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="197" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>364</v>
+        <v>242</v>
       </c>
       <c r="C197" s="4">
+        <v>2016</v>
+      </c>
+      <c r="D197" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E197" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C198" s="4">
         <v>2017</v>
       </c>
-      <c r="D197" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E197" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B198" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C198" s="4">
+      <c r="D198" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E198" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C199" s="4">
         <v>2018</v>
       </c>
-      <c r="D198" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E198" s="4" t="s">
+      <c r="D199" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E199" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B199" s="1" t="s">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B200" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C199" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D199" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E199" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>139</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C200" s="2">
         <v>2018</v>
@@ -4881,47 +4887,64 @@
         <v>9999</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>274</v>
+        <v>137</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C201" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D201" s="2">
         <v>9999</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>137</v>
+        <v>348</v>
       </c>
       <c r="B202" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C202" s="2">
+        <v>2019</v>
+      </c>
+      <c r="D202" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>135</v>
+      </c>
+      <c r="B203" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C202" s="2">
+      <c r="C203" s="2">
         <v>2021</v>
       </c>
-      <c r="D202" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E202" s="2" t="s">
+      <c r="D203" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E203" s="2" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E202">
-    <sortCondition ref="C2:C202"/>
-    <sortCondition ref="E2:E202"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E203">
+    <sortCondition ref="C2:C203"/>
+    <sortCondition ref="E2:E203"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reflects Ken's updated SVGs of 12/23/3030 and 5 addition 'text only' records in the CSV file.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\prototype-historical-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{590C20E0-6708-4859-BAFC-9ED23CFE1496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9480C6E8-0E51-4CC0-901F-96C35301EE51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{48B35B47-D791-4DB0-8E3F-11AF1DC17D23}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="378">
   <si>
     <t>Middlesex Turnpike, opened 1811</t>
   </si>
@@ -1132,13 +1132,40 @@
   </si>
   <si>
     <t>Newburyport commuter rail line (Ipswich-Newburyport)</t>
+  </si>
+  <si>
+    <t>Green_Line_Huntington-1941-1985</t>
+  </si>
+  <si>
+    <t>Green_Line-A-Line-1889-1967</t>
+  </si>
+  <si>
+    <t>Green Line Watertown Branch (A Line)</t>
+  </si>
+  <si>
+    <t>Green Line Arborway (E Line)</t>
+  </si>
+  <si>
+    <t>Stadium Station Red Line</t>
+  </si>
+  <si>
+    <t>Harvard/Brattle Extension Red Line</t>
+  </si>
+  <si>
+    <t>Tremont Street Subway</t>
+  </si>
+  <si>
+    <t>Sliver Line to City Point (original SL3)</t>
+  </si>
+  <si>
+    <t>Elevated Green Line North Station Stop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1150,6 +1177,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1175,7 +1209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1194,6 +1228,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1508,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB246BE0-9101-4910-B137-94A0FD6048BC}">
-  <dimension ref="A1:E203"/>
+  <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A176" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2851,20 +2886,20 @@
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>118</v>
+      <c r="A81" s="7" t="s">
+        <v>370</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>8</v>
+        <v>371</v>
       </c>
       <c r="C81" s="2">
-        <v>1894</v>
+        <v>1889</v>
       </c>
       <c r="D81" s="2">
-        <v>1919</v>
+        <v>1967</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2872,44 +2907,44 @@
         <v>118</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C82" s="2">
         <v>1894</v>
       </c>
       <c r="D82" s="2">
-        <v>9999</v>
+        <v>1919</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>187</v>
+        <v>118</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>307</v>
+        <v>9</v>
       </c>
       <c r="C83" s="2">
-        <v>1897</v>
+        <v>1894</v>
       </c>
       <c r="D83" s="2">
         <v>9999</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C84" s="2">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="D84" s="2">
         <v>9999</v>
@@ -2920,81 +2955,81 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C85" s="2">
+        <v>1898</v>
+      </c>
+      <c r="D85" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C86" s="2">
         <v>1899</v>
       </c>
-      <c r="D85" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>111</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C86" s="2">
-        <v>1901</v>
-      </c>
       <c r="D86" s="2">
-        <v>1987</v>
+        <v>9999</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C87" s="2">
         <v>1901</v>
       </c>
       <c r="D87" s="2">
-        <v>1938</v>
+        <v>1987</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>113</v>
+      <c r="A88" t="s">
+        <v>112</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C88" s="2">
         <v>1901</v>
       </c>
       <c r="D88" s="2">
-        <v>9999</v>
+        <v>1938</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>114</v>
+      <c r="A89" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C89" s="2">
-        <v>1904</v>
+        <v>1901</v>
       </c>
       <c r="D89" s="2">
         <v>9999</v>
@@ -3005,30 +3040,30 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>342</v>
+        <v>118</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>236</v>
+        <v>375</v>
       </c>
       <c r="C90" s="2">
-        <v>1906</v>
+        <v>1901</v>
       </c>
       <c r="D90" s="2">
-        <v>9999</v>
+        <v>1908</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
-        <v>343</v>
+      <c r="A91" t="s">
+        <v>114</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
       <c r="C91" s="2">
-        <v>1907</v>
+        <v>1904</v>
       </c>
       <c r="D91" s="2">
         <v>9999</v>
@@ -3038,31 +3073,31 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>115</v>
+      <c r="A92" s="5" t="s">
+        <v>342</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>15</v>
+        <v>236</v>
       </c>
       <c r="C92" s="2">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="D92" s="2">
-        <v>1987</v>
+        <v>9999</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>165</v>
+      <c r="A93" s="5" t="s">
+        <v>343</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C93" s="2">
-        <v>1912</v>
+        <v>1907</v>
       </c>
       <c r="D93" s="2">
         <v>9999</v>
@@ -3073,30 +3108,30 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>349</v>
+        <v>115</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>310</v>
+        <v>15</v>
       </c>
       <c r="C94" s="2">
-        <v>1912</v>
+        <v>1908</v>
       </c>
       <c r="D94" s="2">
-        <v>9999</v>
+        <v>1987</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>116</v>
+      <c r="A95" t="s">
+        <v>165</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>16</v>
+        <v>309</v>
       </c>
       <c r="C95" s="2">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="D95" s="2">
         <v>9999</v>
@@ -3106,14 +3141,14 @@
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
-        <v>350</v>
+      <c r="A96" t="s">
+        <v>349</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C96" s="2">
-        <v>1915</v>
+        <v>1912</v>
       </c>
       <c r="D96" s="2">
         <v>9999</v>
@@ -3123,17 +3158,17 @@
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>117</v>
+      <c r="A97" t="s">
+        <v>118</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>17</v>
+        <v>377</v>
       </c>
       <c r="C97" s="2">
-        <v>1916</v>
+        <v>1912</v>
       </c>
       <c r="D97" s="2">
-        <v>9999</v>
+        <v>2004</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>88</v>
@@ -3141,13 +3176,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>188</v>
+        <v>116</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>313</v>
+        <v>16</v>
       </c>
       <c r="C98" s="2">
-        <v>1917</v>
+        <v>1914</v>
       </c>
       <c r="D98" s="2">
         <v>9999</v>
@@ -3158,13 +3193,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>189</v>
+        <v>350</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C99" s="2">
-        <v>1918</v>
+        <v>1915</v>
       </c>
       <c r="D99" s="2">
         <v>9999</v>
@@ -3175,33 +3210,33 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>327</v>
+        <v>17</v>
       </c>
       <c r="C100" s="2">
-        <v>1919</v>
+        <v>1916</v>
       </c>
       <c r="D100" s="2">
-        <v>2009</v>
+        <v>9999</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>119</v>
+      <c r="A101" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>18</v>
+        <v>313</v>
       </c>
       <c r="C101" s="2">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="D101" s="2">
-        <v>1975</v>
+        <v>9999</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>88</v>
@@ -3209,13 +3244,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>118</v>
+        <v>189</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>19</v>
+        <v>314</v>
       </c>
       <c r="C102" s="2">
-        <v>1922</v>
+        <v>1918</v>
       </c>
       <c r="D102" s="2">
         <v>9999</v>
@@ -3225,34 +3260,34 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>120</v>
+      <c r="A103" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>21</v>
+        <v>327</v>
       </c>
       <c r="C103" s="2">
-        <v>1923</v>
+        <v>1919</v>
       </c>
       <c r="D103" s="2">
-        <v>9999</v>
+        <v>2009</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>198</v>
+      <c r="A104" t="s">
+        <v>119</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C104" s="2">
-        <v>1927</v>
+        <v>1919</v>
       </c>
       <c r="D104" s="2">
-        <v>9999</v>
+        <v>1975</v>
       </c>
       <c r="E104" s="2" t="s">
         <v>88</v>
@@ -3260,13 +3295,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>199</v>
+        <v>118</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C105" s="2">
-        <v>1928</v>
+        <v>1922</v>
       </c>
       <c r="D105" s="2">
         <v>9999</v>
@@ -3276,85 +3311,85 @@
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>197</v>
+      <c r="A106" t="s">
+        <v>120</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C106" s="2">
-        <v>1929</v>
+        <v>1923</v>
       </c>
       <c r="D106" s="2">
         <v>9999</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>121</v>
+        <v>198</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C107" s="2">
-        <v>1934</v>
+        <v>1927</v>
       </c>
       <c r="D107" s="2">
         <v>9999</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>118</v>
+        <v>199</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>315</v>
+        <v>22</v>
       </c>
       <c r="C108" s="2">
-        <v>1936</v>
+        <v>1928</v>
       </c>
       <c r="D108" s="2">
-        <v>1963</v>
+        <v>9999</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>123</v>
+      <c r="A109" s="5" t="s">
+        <v>197</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C109" s="2">
-        <v>1941</v>
+        <v>1929</v>
       </c>
       <c r="D109" s="2">
         <v>9999</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>25</v>
+        <v>373</v>
       </c>
       <c r="C110" s="2">
-        <v>1941</v>
+        <v>1930</v>
       </c>
       <c r="D110" s="2">
-        <v>9999</v>
+        <v>1983</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>88</v>
@@ -3362,19 +3397,19 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C111" s="2">
-        <v>1943</v>
+        <v>1934</v>
       </c>
       <c r="D111" s="2">
         <v>9999</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3382,67 +3417,67 @@
         <v>118</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="C112" s="2">
-        <v>1947</v>
+        <v>1936</v>
       </c>
       <c r="D112" s="2">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
-        <v>124</v>
+      <c r="A113" t="s">
+        <v>123</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C113" s="2">
-        <v>1950</v>
+        <v>1941</v>
       </c>
       <c r="D113" s="2">
         <v>9999</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>125</v>
+      <c r="A114" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>211</v>
+        <v>25</v>
       </c>
       <c r="C114" s="2">
-        <v>1951</v>
+        <v>1941</v>
       </c>
       <c r="D114" s="2">
         <v>9999</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>175</v>
+      <c r="A115" s="8" t="s">
+        <v>369</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>176</v>
+        <v>372</v>
       </c>
       <c r="C115" s="2">
-        <v>1952</v>
+        <v>1941</v>
       </c>
       <c r="D115" s="2">
-        <v>9999</v>
+        <v>1985</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3450,30 +3485,30 @@
         <v>118</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C116" s="2">
-        <v>1952</v>
+        <v>1943</v>
       </c>
       <c r="D116" s="2">
-        <v>2009</v>
+        <v>9999</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>29</v>
+        <v>326</v>
       </c>
       <c r="C117" s="2">
-        <v>1952</v>
+        <v>1947</v>
       </c>
       <c r="D117" s="2">
-        <v>9999</v>
+        <v>1964</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>88</v>
@@ -3481,13 +3516,13 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C118" s="2">
-        <v>1954</v>
+        <v>1950</v>
       </c>
       <c r="D118" s="2">
         <v>9999</v>
@@ -3497,14 +3532,14 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
-        <v>129</v>
+      <c r="A119" t="s">
+        <v>125</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C119" s="2">
-        <v>1954</v>
+        <v>1951</v>
       </c>
       <c r="D119" s="2">
         <v>9999</v>
@@ -3514,34 +3549,34 @@
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
-        <v>127</v>
+      <c r="A120" t="s">
+        <v>175</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>31</v>
+        <v>176</v>
       </c>
       <c r="C120" s="2">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="D120" s="2">
         <v>9999</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>213</v>
+        <v>30</v>
       </c>
       <c r="C121" s="2">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="D121" s="2">
-        <v>9999</v>
+        <v>2009</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>86</v>
@@ -3549,33 +3584,33 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C122" s="2">
-        <v>1956</v>
+        <v>1952</v>
       </c>
       <c r="D122" s="2">
         <v>9999</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="C123" s="2">
-        <v>1957</v>
+        <v>1954</v>
       </c>
       <c r="D123" s="2">
-        <v>2016</v>
+        <v>9999</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>86</v>
@@ -3583,13 +3618,13 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>362</v>
+        <v>129</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C124" s="2">
-        <v>1957</v>
+        <v>1954</v>
       </c>
       <c r="D124" s="2">
         <v>9999</v>
@@ -3600,30 +3635,30 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>215</v>
+        <v>31</v>
       </c>
       <c r="C125" s="2">
-        <v>1957</v>
+        <v>1954</v>
       </c>
       <c r="D125" s="2">
         <v>9999</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>177</v>
+        <v>130</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>34</v>
+        <v>213</v>
       </c>
       <c r="C126" s="2">
-        <v>1958</v>
+        <v>1955</v>
       </c>
       <c r="D126" s="2">
         <v>9999</v>
@@ -3632,35 +3667,35 @@
         <v>86</v>
       </c>
     </row>
-    <row r="127" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="B127" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C127" s="4">
-        <v>1958</v>
-      </c>
-      <c r="D127" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E127" s="4" t="s">
-        <v>86</v>
+        <v>118</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C127" s="2">
+        <v>1956</v>
+      </c>
+      <c r="D127" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>217</v>
+        <v>82</v>
       </c>
       <c r="C128" s="2">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="D128" s="2">
-        <v>9999</v>
+        <v>2016</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>86</v>
@@ -3668,16 +3703,16 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>118</v>
+        <v>362</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>81</v>
+        <v>214</v>
       </c>
       <c r="C129" s="2">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="D129" s="2">
-        <v>2004</v>
+        <v>9999</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>86</v>
@@ -3685,13 +3720,13 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>80</v>
+        <v>215</v>
       </c>
       <c r="C130" s="2">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="D130" s="2">
         <v>9999</v>
@@ -3702,30 +3737,30 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>132</v>
+        <v>177</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C131" s="2">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="D131" s="2">
         <v>9999</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="132" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>192</v>
+        <v>361</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C132" s="4">
-        <v>1961</v>
+        <v>1958</v>
       </c>
       <c r="D132" s="4">
         <v>9999</v>
@@ -3736,13 +3771,13 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>36</v>
+        <v>217</v>
       </c>
       <c r="C133" s="2">
-        <v>1962</v>
+        <v>1958</v>
       </c>
       <c r="D133" s="2">
         <v>9999</v>
@@ -3752,17 +3787,17 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>164</v>
+      <c r="A134" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>219</v>
+        <v>81</v>
       </c>
       <c r="C134" s="2">
-        <v>1962</v>
+        <v>1959</v>
       </c>
       <c r="D134" s="2">
-        <v>9999</v>
+        <v>2004</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>86</v>
@@ -3770,13 +3805,13 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>37</v>
+        <v>80</v>
       </c>
       <c r="C135" s="2">
-        <v>1962</v>
+        <v>1959</v>
       </c>
       <c r="D135" s="2">
         <v>9999</v>
@@ -3787,47 +3822,47 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="C136" s="2">
-        <v>1963</v>
+        <v>1959</v>
       </c>
       <c r="D136" s="2">
         <v>9999</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>178</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C137" s="2">
-        <v>1964</v>
-      </c>
-      <c r="D137" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E137" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C137" s="4">
+        <v>1961</v>
+      </c>
+      <c r="D137" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E137" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>179</v>
+        <v>133</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C138" s="2">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="D138" s="2">
         <v>9999</v>
@@ -3837,31 +3872,31 @@
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="5" t="s">
-        <v>118</v>
+      <c r="A139" t="s">
+        <v>164</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>324</v>
+        <v>219</v>
       </c>
       <c r="C139" s="2">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="D139" s="2">
         <v>9999</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C140" s="2">
-        <v>1965</v>
+        <v>1962</v>
       </c>
       <c r="D140" s="2">
         <v>9999</v>
@@ -3872,13 +3907,13 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>130</v>
+        <v>190</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C141" s="2">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="D141" s="2">
         <v>9999</v>
@@ -3889,13 +3924,13 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C142" s="2">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="D142" s="2">
         <v>9999</v>
@@ -3905,14 +3940,14 @@
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>162</v>
+      <c r="A143" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C143" s="2">
-        <v>1966</v>
+        <v>1964</v>
       </c>
       <c r="D143" s="2">
         <v>9999</v>
@@ -3922,65 +3957,65 @@
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>161</v>
+      <c r="A144" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>41</v>
+        <v>324</v>
       </c>
       <c r="C144" s="2">
-        <v>1969</v>
+        <v>1964</v>
       </c>
       <c r="D144" s="2">
         <v>9999</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B145" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C145" s="4">
-        <v>1970</v>
-      </c>
-      <c r="D145" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E145" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C145" s="2">
+        <v>1965</v>
+      </c>
+      <c r="D145" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E145" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>351</v>
+        <v>130</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>42</v>
+        <v>222</v>
       </c>
       <c r="C146" s="2">
-        <v>1971</v>
+        <v>1965</v>
       </c>
       <c r="D146" s="2">
         <v>9999</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>43</v>
+        <v>223</v>
       </c>
       <c r="C147" s="2">
-        <v>1973</v>
+        <v>1965</v>
       </c>
       <c r="D147" s="2">
         <v>9999</v>
@@ -3990,343 +4025,343 @@
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
-        <v>118</v>
+      <c r="A148" t="s">
+        <v>162</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C148" s="2">
-        <v>1974</v>
+        <v>1966</v>
       </c>
       <c r="D148" s="2">
         <v>9999</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C149" s="2">
-        <v>1975</v>
+        <v>1969</v>
       </c>
       <c r="D149" s="2">
         <v>9999</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="150" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
-        <v>118</v>
+      <c r="A150" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>57</v>
+        <v>182</v>
       </c>
       <c r="C150" s="4">
-        <v>1975</v>
+        <v>1970</v>
       </c>
       <c r="D150" s="4">
         <v>9999</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B151" s="5" t="s">
-        <v>322</v>
-      </c>
-      <c r="C151" s="4">
-        <v>1975</v>
-      </c>
-      <c r="D151" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E151" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C151" s="2">
+        <v>1971</v>
+      </c>
+      <c r="D151" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E151" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="152" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B152" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C152" s="4">
-        <v>1975</v>
-      </c>
-      <c r="D152" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E152" s="4" t="s">
-        <v>88</v>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>160</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C152" s="2">
+        <v>1973</v>
+      </c>
+      <c r="D152" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>344</v>
+        <v>118</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>237</v>
+        <v>44</v>
       </c>
       <c r="C153" s="2">
-        <v>1979</v>
+        <v>1974</v>
       </c>
       <c r="D153" s="2">
         <v>9999</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="B154" s="5" t="s">
-        <v>323</v>
-      </c>
-      <c r="C154" s="4">
-        <v>1980</v>
-      </c>
-      <c r="D154" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E154" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>159</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C154" s="2">
+        <v>1975</v>
+      </c>
+      <c r="D154" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C155" s="4">
+        <v>1975</v>
+      </c>
+      <c r="D155" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E155" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C156" s="4">
+        <v>1975</v>
+      </c>
+      <c r="D156" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E156" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C155" s="2">
-        <v>1984</v>
-      </c>
-      <c r="D155" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E155" s="2" t="s">
+    <row r="157" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C157" s="4">
+        <v>1975</v>
+      </c>
+      <c r="D157" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E157" s="4" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C156" s="2">
-        <v>1985</v>
-      </c>
-      <c r="D156" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E156" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="C157" s="2">
-        <v>1987</v>
-      </c>
-      <c r="D157" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E157" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>157</v>
+        <v>344</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>47</v>
+        <v>237</v>
       </c>
       <c r="C158" s="2">
-        <v>1987</v>
+        <v>1979</v>
       </c>
       <c r="D158" s="2">
         <v>9999</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>58</v>
+        <v>374</v>
       </c>
       <c r="C159" s="2">
-        <v>1992</v>
+        <v>1979</v>
       </c>
       <c r="D159" s="2">
-        <v>9999</v>
+        <v>1983</v>
       </c>
       <c r="E159" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C160" s="4">
+        <v>1980</v>
+      </c>
+      <c r="D160" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E160" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C161" s="2">
+        <v>1984</v>
+      </c>
+      <c r="D161" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C162" s="2">
+        <v>1985</v>
+      </c>
+      <c r="D162" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C163" s="2">
+        <v>1987</v>
+      </c>
+      <c r="D163" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E163" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="B160" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="C160" s="2">
-        <v>1992</v>
-      </c>
-      <c r="D160" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E160" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B161" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="C161" s="4">
-        <v>1993</v>
-      </c>
-      <c r="D161" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E161" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C162" s="4">
-        <v>1994</v>
-      </c>
-      <c r="D162" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E162" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>345</v>
-      </c>
-      <c r="B163" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C163" s="2">
-        <v>1994</v>
-      </c>
-      <c r="D163" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E163" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B164" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C164" s="4">
-        <v>1995</v>
-      </c>
-      <c r="D164" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E164" s="4" t="s">
-        <v>86</v>
+        <v>157</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C164" s="2">
+        <v>1987</v>
+      </c>
+      <c r="D164" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C165" s="2">
-        <v>1995</v>
+        <v>1992</v>
       </c>
       <c r="D165" s="2">
         <v>9999</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C166" s="2">
+        <v>1992</v>
+      </c>
+      <c r="D166" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B166" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C166" s="2">
-        <v>1995</v>
-      </c>
-      <c r="D166" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
-        <v>365</v>
-      </c>
-      <c r="B167" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C167" s="2">
-        <v>1997</v>
-      </c>
-      <c r="D167" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>89</v>
+      <c r="B167" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C167" s="4">
+        <v>1993</v>
+      </c>
+      <c r="D167" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E167" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="168" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -4334,27 +4369,27 @@
         <v>118</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C168" s="4">
-        <v>1998</v>
+        <v>1994</v>
       </c>
       <c r="D168" s="4">
         <v>9999</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C169" s="2">
-        <v>1998</v>
+        <v>1994</v>
       </c>
       <c r="D169" s="2">
         <v>9999</v>
@@ -4363,134 +4398,134 @@
         <v>89</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>346</v>
-      </c>
-      <c r="B170" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C170" s="2">
-        <v>1999</v>
-      </c>
-      <c r="D170" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E170" s="2" t="s">
-        <v>89</v>
+    <row r="170" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C170" s="4">
+        <v>1995</v>
+      </c>
+      <c r="D170" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E170" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>154</v>
+      <c r="A171" s="5" t="s">
+        <v>155</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C171" s="2">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="D171" s="2">
         <v>9999</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B172" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C172" s="4">
-        <v>2002</v>
-      </c>
-      <c r="D172" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E172" s="4" t="s">
-        <v>86</v>
+      <c r="B172" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C172" s="2">
+        <v>1995</v>
+      </c>
+      <c r="D172" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>153</v>
+      <c r="A173" s="5" t="s">
+        <v>365</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>53</v>
+        <v>239</v>
       </c>
       <c r="C173" s="2">
-        <v>2002</v>
+        <v>1997</v>
       </c>
       <c r="D173" s="2">
         <v>9999</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>152</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C174" s="2">
-        <v>2003</v>
-      </c>
-      <c r="D174" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E174" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C174" s="4">
+        <v>1998</v>
+      </c>
+      <c r="D174" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E174" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="175" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B175" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C175" s="4">
-        <v>2003</v>
-      </c>
-      <c r="D175" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E175" s="4" t="s">
-        <v>86</v>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>366</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C175" s="2">
+        <v>1998</v>
+      </c>
+      <c r="D175" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>151</v>
+        <v>346</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>61</v>
+        <v>241</v>
       </c>
       <c r="C176" s="2">
-        <v>2003</v>
+        <v>1999</v>
       </c>
       <c r="D176" s="2">
         <v>9999</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>317</v>
+        <v>55</v>
       </c>
       <c r="C177" s="2">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="D177" s="2">
         <v>9999</v>
@@ -4499,49 +4534,49 @@
         <v>92</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B178" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C178" s="2">
-        <v>2005</v>
-      </c>
-      <c r="D178" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E178" s="2" t="s">
+      <c r="B178" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C178" s="4">
+        <v>2002</v>
+      </c>
+      <c r="D178" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E178" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="5" t="s">
-        <v>118</v>
+      <c r="A179" t="s">
+        <v>153</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C179" s="2">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="D179" s="2">
         <v>9999</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>318</v>
+        <v>60</v>
       </c>
       <c r="C180" s="2">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="D180" s="2">
         <v>9999</v>
@@ -4550,89 +4585,89 @@
         <v>92</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C181" s="2">
-        <v>2007</v>
-      </c>
-      <c r="D181" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E181" s="2" t="s">
-        <v>92</v>
+        <v>118</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C181" s="4">
+        <v>2003</v>
+      </c>
+      <c r="D181" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E181" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" s="5" t="s">
-        <v>347</v>
+      <c r="A182" t="s">
+        <v>151</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>191</v>
+        <v>61</v>
       </c>
       <c r="C182" s="2">
-        <v>2007</v>
+        <v>2003</v>
       </c>
       <c r="D182" s="2">
         <v>9999</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>66</v>
+        <v>376</v>
       </c>
       <c r="C183" s="2">
-        <v>2008</v>
+        <v>2004</v>
       </c>
       <c r="D183" s="2">
-        <v>9999</v>
+        <v>2009</v>
       </c>
       <c r="E183" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>150</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C184" s="2">
+        <v>2005</v>
+      </c>
+      <c r="D184" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E184" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="184" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="5" t="s">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B184" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C184" s="4">
-        <v>2008</v>
-      </c>
-      <c r="D184" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E184" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>139</v>
-      </c>
       <c r="B185" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C185" s="2">
-        <v>2009</v>
+        <v>2005</v>
       </c>
       <c r="D185" s="2">
         <v>9999</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4640,78 +4675,78 @@
         <v>118</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>319</v>
+        <v>62</v>
       </c>
       <c r="C186" s="2">
-        <v>2009</v>
+        <v>2005</v>
       </c>
       <c r="D186" s="2">
         <v>9999</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>68</v>
+        <v>318</v>
       </c>
       <c r="C187" s="2">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="D187" s="2">
         <v>9999</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B188" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C188" s="4">
-        <v>2010</v>
-      </c>
-      <c r="D188" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E188" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C188" s="2">
+        <v>2007</v>
+      </c>
+      <c r="D188" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E188" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>141</v>
+      <c r="A189" s="5" t="s">
+        <v>347</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>70</v>
+        <v>191</v>
       </c>
       <c r="C189" s="2">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="D189" s="2">
         <v>9999</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="5" t="s">
-        <v>147</v>
+      <c r="A190" t="s">
+        <v>142</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>320</v>
+        <v>66</v>
       </c>
       <c r="C190" s="2">
-        <v>2012</v>
+        <v>2008</v>
       </c>
       <c r="D190" s="2">
         <v>9999</v>
@@ -4720,32 +4755,32 @@
         <v>92</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>138</v>
-      </c>
-      <c r="B191" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C191" s="2">
-        <v>2013</v>
-      </c>
-      <c r="D191" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E191" s="2" t="s">
+    <row r="191" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C191" s="4">
+        <v>2008</v>
+      </c>
+      <c r="D191" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E191" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C192" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="D192" s="2">
         <v>9999</v>
@@ -4754,66 +4789,66 @@
         <v>92</v>
       </c>
     </row>
-    <row r="193" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B193" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="C193" s="4">
-        <v>2014</v>
-      </c>
-      <c r="D193" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E193" s="4" t="s">
+      <c r="B193" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C193" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D193" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E193" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>140</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C194" s="2">
+        <v>2009</v>
+      </c>
+      <c r="D194" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E194" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B194" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C194" s="2">
-        <v>2015</v>
-      </c>
-      <c r="D194" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E194" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A195" t="s">
-        <v>145</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C195" s="2">
-        <v>2015</v>
-      </c>
-      <c r="D195" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E195" s="2" t="s">
+    <row r="195" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C195" s="4">
+        <v>2010</v>
+      </c>
+      <c r="D195" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E195" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C196" s="2">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="D196" s="2">
         <v>9999</v>
@@ -4822,100 +4857,100 @@
         <v>92</v>
       </c>
     </row>
-    <row r="197" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C197" s="2">
+        <v>2012</v>
+      </c>
+      <c r="D197" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E197" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>138</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C198" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D198" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E198" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>143</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C199" s="2">
+        <v>2014</v>
+      </c>
+      <c r="D199" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B197" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C197" s="4">
-        <v>2016</v>
-      </c>
-      <c r="D197" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E197" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B198" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="C198" s="4">
-        <v>2017</v>
-      </c>
-      <c r="D198" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E198" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B199" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C199" s="4">
-        <v>2018</v>
-      </c>
-      <c r="D199" s="4">
-        <v>9999</v>
-      </c>
-      <c r="E199" s="4" t="s">
+      <c r="B200" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C200" s="4">
+        <v>2014</v>
+      </c>
+      <c r="D200" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E200" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C201" s="2">
+        <v>2015</v>
+      </c>
+      <c r="D201" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E201" s="2" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C200" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D200" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E200" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>137</v>
-      </c>
-      <c r="B201" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C201" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D201" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E201" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>348</v>
+        <v>145</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C202" s="2">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="D202" s="2">
         <v>9999</v>
@@ -4926,25 +4961,144 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>146</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C203" s="2">
+        <v>2015</v>
+      </c>
+      <c r="D203" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C204" s="4">
+        <v>2016</v>
+      </c>
+      <c r="D204" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E204" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C205" s="4">
+        <v>2017</v>
+      </c>
+      <c r="D205" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E205" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C206" s="4">
+        <v>2018</v>
+      </c>
+      <c r="D206" s="4">
+        <v>9999</v>
+      </c>
+      <c r="E206" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C207" s="2">
+        <v>2018</v>
+      </c>
+      <c r="D207" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>137</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C208" s="2">
+        <v>2018</v>
+      </c>
+      <c r="D208" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>348</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C209" s="2">
+        <v>2019</v>
+      </c>
+      <c r="D209" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
         <v>135</v>
       </c>
-      <c r="B203" s="1" t="s">
+      <c r="B210" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C203" s="2">
+      <c r="C210" s="2">
         <v>2021</v>
       </c>
-      <c r="D203" s="2">
-        <v>9999</v>
-      </c>
-      <c r="E203" s="2" t="s">
+      <c r="D210" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E210" s="2" t="s">
         <v>88</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E203">
-    <sortCondition ref="C2:C203"/>
-    <sortCondition ref="E2:E203"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E210">
+    <sortCondition ref="C2:C210"/>
+    <sortCondition ref="E2:E210"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed empty 'type' field for Newburyport-CR-1839 record.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\prototype-historical-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9480C6E8-0E51-4CC0-901F-96C35301EE51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B421C5ED-D56D-4999-9966-FB46CA835A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{48B35B47-D791-4DB0-8E3F-11AF1DC17D23}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="378">
   <si>
     <t>Middlesex Turnpike, opened 1811</t>
   </si>
@@ -1545,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB246BE0-9101-4910-B137-94A0FD6048BC}">
   <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,6 +2068,9 @@
       <c r="D32" s="2">
         <v>9999</v>
       </c>
+      <c r="E32" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">

</xml_diff>

<commit_message>
Reflects change in layer name: 'I-93_SE_Expressway_Rt.3_Rt.24_I-95' to 'I-93_SE_Expressway_Rt_3_Rt_24_I-95'.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\prototype-historical-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D70EBD5-74B4-43E8-B282-69E10304CA44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC20B3CF-ED60-4AAC-975E-358950A5C816}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feature_timeline" sheetId="1" r:id="rId1"/>
@@ -751,9 +751,6 @@
     <t>Interstate 93 (Fort Hill-SE Expressway)</t>
   </si>
   <si>
-    <t>I-93_SE_Expressway_Rt.3_Rt.24_I-95</t>
-  </si>
-  <si>
     <t>Interstate 93 (SE Expressway-Route 3-Route 24-I-95)</t>
   </si>
   <si>
@@ -1151,12 +1148,15 @@
   </si>
   <si>
     <t>Green Line to Medford (GLX)</t>
+  </si>
+  <si>
+    <t>I-93_SE_Expressway_Rt_3_Rt_24_I-95</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1990,10 +1990,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="A133" sqref="A133"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4202,10 +4204,10 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>376</v>
+      </c>
+      <c r="B132" t="s">
         <v>243</v>
-      </c>
-      <c r="B132" t="s">
-        <v>244</v>
       </c>
       <c r="C132">
         <v>1958</v>
@@ -4219,10 +4221,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>244</v>
+      </c>
+      <c r="B133" t="s">
         <v>245</v>
-      </c>
-      <c r="B133" t="s">
-        <v>246</v>
       </c>
       <c r="C133">
         <v>1958</v>
@@ -4239,7 +4241,7 @@
         <v>33</v>
       </c>
       <c r="B134" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C134">
         <v>1959</v>
@@ -4256,7 +4258,7 @@
         <v>33</v>
       </c>
       <c r="B135" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C135">
         <v>1959</v>
@@ -4270,10 +4272,10 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>248</v>
+      </c>
+      <c r="B136" t="s">
         <v>249</v>
-      </c>
-      <c r="B136" t="s">
-        <v>250</v>
       </c>
       <c r="C136">
         <v>1959</v>
@@ -4287,10 +4289,10 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>250</v>
+      </c>
+      <c r="B137" t="s">
         <v>251</v>
-      </c>
-      <c r="B137" t="s">
-        <v>252</v>
       </c>
       <c r="C137">
         <v>1961</v>
@@ -4304,10 +4306,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>252</v>
+      </c>
+      <c r="B138" t="s">
         <v>253</v>
-      </c>
-      <c r="B138" t="s">
-        <v>254</v>
       </c>
       <c r="C138">
         <v>1962</v>
@@ -4321,10 +4323,10 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>254</v>
+      </c>
+      <c r="B139" t="s">
         <v>255</v>
-      </c>
-      <c r="B139" t="s">
-        <v>256</v>
       </c>
       <c r="C139">
         <v>1962</v>
@@ -4338,10 +4340,10 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>256</v>
+      </c>
+      <c r="B140" t="s">
         <v>257</v>
-      </c>
-      <c r="B140" t="s">
-        <v>258</v>
       </c>
       <c r="C140">
         <v>1962</v>
@@ -4355,10 +4357,10 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>258</v>
+      </c>
+      <c r="B141" t="s">
         <v>259</v>
-      </c>
-      <c r="B141" t="s">
-        <v>260</v>
       </c>
       <c r="C141">
         <v>1963</v>
@@ -4372,10 +4374,10 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
+        <v>260</v>
+      </c>
+      <c r="B142" t="s">
         <v>261</v>
-      </c>
-      <c r="B142" t="s">
-        <v>262</v>
       </c>
       <c r="C142">
         <v>1964</v>
@@ -4389,10 +4391,10 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
+        <v>262</v>
+      </c>
+      <c r="B143" t="s">
         <v>263</v>
-      </c>
-      <c r="B143" t="s">
-        <v>264</v>
       </c>
       <c r="C143">
         <v>1964</v>
@@ -4409,7 +4411,7 @@
         <v>33</v>
       </c>
       <c r="B144" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C144">
         <v>1964</v>
@@ -4423,10 +4425,10 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>265</v>
+      </c>
+      <c r="B145" t="s">
         <v>266</v>
-      </c>
-      <c r="B145" t="s">
-        <v>267</v>
       </c>
       <c r="C145">
         <v>1965</v>
@@ -4443,7 +4445,7 @@
         <v>233</v>
       </c>
       <c r="B146" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C146">
         <v>1965</v>
@@ -4457,10 +4459,10 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>268</v>
+      </c>
+      <c r="B147" t="s">
         <v>269</v>
-      </c>
-      <c r="B147" t="s">
-        <v>270</v>
       </c>
       <c r="C147">
         <v>1965</v>
@@ -4474,10 +4476,10 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
+        <v>270</v>
+      </c>
+      <c r="B148" t="s">
         <v>271</v>
-      </c>
-      <c r="B148" t="s">
-        <v>272</v>
       </c>
       <c r="C148">
         <v>1966</v>
@@ -4491,10 +4493,10 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>272</v>
+      </c>
+      <c r="B149" t="s">
         <v>273</v>
-      </c>
-      <c r="B149" t="s">
-        <v>274</v>
       </c>
       <c r="C149">
         <v>1969</v>
@@ -4508,10 +4510,10 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
+        <v>274</v>
+      </c>
+      <c r="B150" t="s">
         <v>275</v>
-      </c>
-      <c r="B150" t="s">
-        <v>276</v>
       </c>
       <c r="C150">
         <v>1970</v>
@@ -4525,10 +4527,10 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
+        <v>276</v>
+      </c>
+      <c r="B151" t="s">
         <v>277</v>
-      </c>
-      <c r="B151" t="s">
-        <v>278</v>
       </c>
       <c r="C151">
         <v>1971</v>
@@ -4542,10 +4544,10 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
+        <v>278</v>
+      </c>
+      <c r="B152" t="s">
         <v>279</v>
-      </c>
-      <c r="B152" t="s">
-        <v>280</v>
       </c>
       <c r="C152">
         <v>1973</v>
@@ -4562,7 +4564,7 @@
         <v>33</v>
       </c>
       <c r="B153" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C153">
         <v>1974</v>
@@ -4576,10 +4578,10 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>281</v>
+      </c>
+      <c r="B154" t="s">
         <v>282</v>
-      </c>
-      <c r="B154" t="s">
-        <v>283</v>
       </c>
       <c r="C154">
         <v>1975</v>
@@ -4588,7 +4590,7 @@
         <v>9999</v>
       </c>
       <c r="E154" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -4596,7 +4598,7 @@
         <v>33</v>
       </c>
       <c r="B155" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C155">
         <v>1975</v>
@@ -4605,15 +4607,15 @@
         <v>9999</v>
       </c>
       <c r="E155" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>285</v>
+      </c>
+      <c r="B156" t="s">
         <v>286</v>
-      </c>
-      <c r="B156" t="s">
-        <v>287</v>
       </c>
       <c r="C156">
         <v>1975</v>
@@ -4627,10 +4629,10 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B157" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C157">
         <v>1975</v>
@@ -4644,10 +4646,10 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>288</v>
+      </c>
+      <c r="B158" t="s">
         <v>289</v>
-      </c>
-      <c r="B158" t="s">
-        <v>290</v>
       </c>
       <c r="C158">
         <v>1979</v>
@@ -4664,7 +4666,7 @@
         <v>33</v>
       </c>
       <c r="B159" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C159">
         <v>1979</v>
@@ -4678,10 +4680,10 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>291</v>
+      </c>
+      <c r="B160" t="s">
         <v>292</v>
-      </c>
-      <c r="B160" t="s">
-        <v>293</v>
       </c>
       <c r="C160">
         <v>1980</v>
@@ -4695,10 +4697,10 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
+        <v>293</v>
+      </c>
+      <c r="B161" t="s">
         <v>294</v>
-      </c>
-      <c r="B161" t="s">
-        <v>295</v>
       </c>
       <c r="C161">
         <v>1984</v>
@@ -4712,10 +4714,10 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>295</v>
+      </c>
+      <c r="B162" t="s">
         <v>296</v>
-      </c>
-      <c r="B162" t="s">
-        <v>297</v>
       </c>
       <c r="C162">
         <v>1985</v>
@@ -4729,10 +4731,10 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>297</v>
+      </c>
+      <c r="B163" t="s">
         <v>298</v>
-      </c>
-      <c r="B163" t="s">
-        <v>299</v>
       </c>
       <c r="C163">
         <v>1987</v>
@@ -4741,15 +4743,15 @@
         <v>9999</v>
       </c>
       <c r="E163" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
+        <v>299</v>
+      </c>
+      <c r="B164" t="s">
         <v>300</v>
-      </c>
-      <c r="B164" t="s">
-        <v>301</v>
       </c>
       <c r="C164">
         <v>1987</v>
@@ -4763,10 +4765,10 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
+        <v>301</v>
+      </c>
+      <c r="B165" t="s">
         <v>302</v>
-      </c>
-      <c r="B165" t="s">
-        <v>303</v>
       </c>
       <c r="C165">
         <v>1992</v>
@@ -4775,15 +4777,15 @@
         <v>9999</v>
       </c>
       <c r="E165" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
+        <v>303</v>
+      </c>
+      <c r="B166" t="s">
         <v>304</v>
-      </c>
-      <c r="B166" t="s">
-        <v>305</v>
       </c>
       <c r="C166">
         <v>1992</v>
@@ -4792,7 +4794,7 @@
         <v>9999</v>
       </c>
       <c r="E166" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -4800,7 +4802,7 @@
         <v>33</v>
       </c>
       <c r="B167" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C167">
         <v>1993</v>
@@ -4817,7 +4819,7 @@
         <v>33</v>
       </c>
       <c r="B168" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C168">
         <v>1994</v>
@@ -4831,10 +4833,10 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
+        <v>307</v>
+      </c>
+      <c r="B169" t="s">
         <v>308</v>
-      </c>
-      <c r="B169" t="s">
-        <v>309</v>
       </c>
       <c r="C169">
         <v>1994</v>
@@ -4851,7 +4853,7 @@
         <v>33</v>
       </c>
       <c r="B170" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C170">
         <v>1995</v>
@@ -4865,10 +4867,10 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>310</v>
+      </c>
+      <c r="B171" t="s">
         <v>311</v>
-      </c>
-      <c r="B171" t="s">
-        <v>312</v>
       </c>
       <c r="C171">
         <v>1995</v>
@@ -4885,7 +4887,7 @@
         <v>33</v>
       </c>
       <c r="B172" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C172">
         <v>1995</v>
@@ -4899,10 +4901,10 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
+        <v>313</v>
+      </c>
+      <c r="B173" t="s">
         <v>314</v>
-      </c>
-      <c r="B173" t="s">
-        <v>315</v>
       </c>
       <c r="C173">
         <v>1997</v>
@@ -4919,7 +4921,7 @@
         <v>33</v>
       </c>
       <c r="B174" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C174">
         <v>1998</v>
@@ -4928,15 +4930,15 @@
         <v>9999</v>
       </c>
       <c r="E174" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
+        <v>316</v>
+      </c>
+      <c r="B175" t="s">
         <v>317</v>
-      </c>
-      <c r="B175" t="s">
-        <v>318</v>
       </c>
       <c r="C175">
         <v>1998</v>
@@ -4950,7 +4952,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B176" t="s">
         <v>60</v>
@@ -4967,10 +4969,10 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>319</v>
+      </c>
+      <c r="B177" t="s">
         <v>320</v>
-      </c>
-      <c r="B177" t="s">
-        <v>321</v>
       </c>
       <c r="C177">
         <v>2002</v>
@@ -4979,7 +4981,7 @@
         <v>9999</v>
       </c>
       <c r="E177" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4987,7 +4989,7 @@
         <v>33</v>
       </c>
       <c r="B178" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C178">
         <v>2002</v>
@@ -5001,10 +5003,10 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>322</v>
+      </c>
+      <c r="B179" t="s">
         <v>323</v>
-      </c>
-      <c r="B179" t="s">
-        <v>324</v>
       </c>
       <c r="C179">
         <v>2002</v>
@@ -5018,10 +5020,10 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>324</v>
+      </c>
+      <c r="B180" t="s">
         <v>325</v>
-      </c>
-      <c r="B180" t="s">
-        <v>326</v>
       </c>
       <c r="C180">
         <v>2003</v>
@@ -5030,7 +5032,7 @@
         <v>9999</v>
       </c>
       <c r="E180" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -5038,7 +5040,7 @@
         <v>33</v>
       </c>
       <c r="B181" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C181">
         <v>2003</v>
@@ -5052,10 +5054,10 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>327</v>
+      </c>
+      <c r="B182" t="s">
         <v>328</v>
-      </c>
-      <c r="B182" t="s">
-        <v>329</v>
       </c>
       <c r="C182">
         <v>2003</v>
@@ -5072,7 +5074,7 @@
         <v>33</v>
       </c>
       <c r="B183" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C183">
         <v>2004</v>
@@ -5086,10 +5088,10 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>330</v>
+      </c>
+      <c r="B184" t="s">
         <v>331</v>
-      </c>
-      <c r="B184" t="s">
-        <v>332</v>
       </c>
       <c r="C184">
         <v>2005</v>
@@ -5098,7 +5100,7 @@
         <v>9999</v>
       </c>
       <c r="E184" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5106,7 +5108,7 @@
         <v>33</v>
       </c>
       <c r="B185" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C185">
         <v>2005</v>
@@ -5123,7 +5125,7 @@
         <v>33</v>
       </c>
       <c r="B186" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C186">
         <v>2005</v>
@@ -5137,10 +5139,10 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>334</v>
+      </c>
+      <c r="B187" t="s">
         <v>335</v>
-      </c>
-      <c r="B187" t="s">
-        <v>336</v>
       </c>
       <c r="C187">
         <v>2006</v>
@@ -5149,15 +5151,15 @@
         <v>9999</v>
       </c>
       <c r="E187" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>336</v>
+      </c>
+      <c r="B188" t="s">
         <v>337</v>
-      </c>
-      <c r="B188" t="s">
-        <v>338</v>
       </c>
       <c r="C188">
         <v>2007</v>
@@ -5166,15 +5168,15 @@
         <v>9999</v>
       </c>
       <c r="E188" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>338</v>
+      </c>
+      <c r="B189" t="s">
         <v>339</v>
-      </c>
-      <c r="B189" t="s">
-        <v>340</v>
       </c>
       <c r="C189">
         <v>2007</v>
@@ -5188,10 +5190,10 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>340</v>
+      </c>
+      <c r="B190" t="s">
         <v>341</v>
-      </c>
-      <c r="B190" t="s">
-        <v>342</v>
       </c>
       <c r="C190">
         <v>2008</v>
@@ -5200,7 +5202,7 @@
         <v>9999</v>
       </c>
       <c r="E190" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5208,7 +5210,7 @@
         <v>33</v>
       </c>
       <c r="B191" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C191">
         <v>2008</v>
@@ -5217,15 +5219,15 @@
         <v>9999</v>
       </c>
       <c r="E191" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>343</v>
+      </c>
+      <c r="B192" t="s">
         <v>344</v>
-      </c>
-      <c r="B192" t="s">
-        <v>345</v>
       </c>
       <c r="C192">
         <v>2009</v>
@@ -5234,7 +5236,7 @@
         <v>9999</v>
       </c>
       <c r="E192" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5242,7 +5244,7 @@
         <v>33</v>
       </c>
       <c r="B193" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C193">
         <v>2009</v>
@@ -5256,10 +5258,10 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
+        <v>346</v>
+      </c>
+      <c r="B194" t="s">
         <v>347</v>
-      </c>
-      <c r="B194" t="s">
-        <v>348</v>
       </c>
       <c r="C194">
         <v>2009</v>
@@ -5276,7 +5278,7 @@
         <v>33</v>
       </c>
       <c r="B195" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C195">
         <v>2010</v>
@@ -5285,15 +5287,15 @@
         <v>9999</v>
       </c>
       <c r="E195" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
+        <v>349</v>
+      </c>
+      <c r="B196" t="s">
         <v>350</v>
-      </c>
-      <c r="B196" t="s">
-        <v>351</v>
       </c>
       <c r="C196">
         <v>2012</v>
@@ -5302,15 +5304,15 @@
         <v>9999</v>
       </c>
       <c r="E196" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>351</v>
+      </c>
+      <c r="B197" t="s">
         <v>352</v>
-      </c>
-      <c r="B197" t="s">
-        <v>353</v>
       </c>
       <c r="C197">
         <v>2012</v>
@@ -5319,15 +5321,15 @@
         <v>9999</v>
       </c>
       <c r="E197" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
+        <v>353</v>
+      </c>
+      <c r="B198" t="s">
         <v>354</v>
-      </c>
-      <c r="B198" t="s">
-        <v>355</v>
       </c>
       <c r="C198">
         <v>2013</v>
@@ -5336,15 +5338,15 @@
         <v>9999</v>
       </c>
       <c r="E198" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>355</v>
+      </c>
+      <c r="B199" t="s">
         <v>356</v>
-      </c>
-      <c r="B199" t="s">
-        <v>357</v>
       </c>
       <c r="C199">
         <v>2014</v>
@@ -5353,7 +5355,7 @@
         <v>9999</v>
       </c>
       <c r="E199" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -5361,7 +5363,7 @@
         <v>33</v>
       </c>
       <c r="B200" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C200">
         <v>2014</v>
@@ -5375,10 +5377,10 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
+        <v>358</v>
+      </c>
+      <c r="B201" t="s">
         <v>359</v>
-      </c>
-      <c r="B201" t="s">
-        <v>360</v>
       </c>
       <c r="C201">
         <v>2015</v>
@@ -5387,15 +5389,15 @@
         <v>9999</v>
       </c>
       <c r="E201" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
+        <v>360</v>
+      </c>
+      <c r="B202" t="s">
         <v>361</v>
-      </c>
-      <c r="B202" t="s">
-        <v>362</v>
       </c>
       <c r="C202">
         <v>2015</v>
@@ -5404,15 +5406,15 @@
         <v>9999</v>
       </c>
       <c r="E202" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>362</v>
+      </c>
+      <c r="B203" t="s">
         <v>363</v>
-      </c>
-      <c r="B203" t="s">
-        <v>364</v>
       </c>
       <c r="C203">
         <v>2015</v>
@@ -5421,7 +5423,7 @@
         <v>9999</v>
       </c>
       <c r="E203" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5429,7 +5431,7 @@
         <v>33</v>
       </c>
       <c r="B204" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C204">
         <v>2016</v>
@@ -5446,7 +5448,7 @@
         <v>33</v>
       </c>
       <c r="B205" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C205">
         <v>2017</v>
@@ -5460,10 +5462,10 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>366</v>
+      </c>
+      <c r="B206" t="s">
         <v>367</v>
-      </c>
-      <c r="B206" t="s">
-        <v>368</v>
       </c>
       <c r="C206">
         <v>2018</v>
@@ -5472,15 +5474,15 @@
         <v>9999</v>
       </c>
       <c r="E206" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
+        <v>368</v>
+      </c>
+      <c r="B207" t="s">
         <v>369</v>
-      </c>
-      <c r="B207" t="s">
-        <v>370</v>
       </c>
       <c r="C207">
         <v>2018</v>
@@ -5489,15 +5491,15 @@
         <v>9999</v>
       </c>
       <c r="E207" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>370</v>
+      </c>
+      <c r="B208" t="s">
         <v>371</v>
-      </c>
-      <c r="B208" t="s">
-        <v>372</v>
       </c>
       <c r="C208">
         <v>2018</v>
@@ -5511,10 +5513,10 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
+        <v>372</v>
+      </c>
+      <c r="B209" t="s">
         <v>373</v>
-      </c>
-      <c r="B209" t="s">
-        <v>374</v>
       </c>
       <c r="C209">
         <v>2019</v>
@@ -5523,15 +5525,15 @@
         <v>9999</v>
       </c>
       <c r="E209" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
+        <v>374</v>
+      </c>
+      <c r="B210" t="s">
         <v>375</v>
-      </c>
-      <c r="B210" t="s">
-        <v>376</v>
       </c>
       <c r="C210">
         <v>2021</v>

</xml_diff>

<commit_message>
Added and populated column indicating reopening.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\prototype-historical-map\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kend/Documents/General Maps/Time Line/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC20B3CF-ED60-4AAC-975E-358950A5C816}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E494E7C-EF1A-A848-8FC6-D8FE521B334C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feature_timeline" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="379">
   <si>
     <t>layer_name</t>
   </si>
@@ -1151,6 +1151,12 @@
   </si>
   <si>
     <t>I-93_SE_Expressway_Rt_3_Rt_24_I-95</t>
+  </si>
+  <si>
+    <t>reopening</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -1991,21 +1997,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E210"/>
+  <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="F176" sqref="F176"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2021,8 +2028,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2036,7 +2046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2050,7 +2060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2064,7 +2074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2078,7 +2088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2092,7 +2102,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2106,7 +2116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2120,7 +2130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2134,7 +2144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2148,7 +2158,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2162,7 +2172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2179,7 +2189,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2196,7 +2206,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2213,7 +2223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2230,7 +2240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2247,7 +2257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -2264,7 +2274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2281,7 +2291,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2298,7 +2308,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2315,7 +2325,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -2332,7 +2342,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2349,7 +2359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2366,7 +2376,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2383,7 +2393,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -2400,7 +2410,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -2417,7 +2427,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -2434,7 +2444,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -2451,7 +2461,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2468,7 +2478,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -2485,7 +2495,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -2502,7 +2512,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -2519,7 +2529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -2536,7 +2546,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2553,7 +2563,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2570,7 +2580,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2587,7 +2597,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -2604,7 +2614,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -2621,7 +2631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -2638,7 +2648,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -2655,7 +2665,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -2672,7 +2682,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -2689,7 +2699,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -2706,7 +2716,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -2723,7 +2733,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -2740,7 +2750,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -2757,7 +2767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -2774,7 +2784,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2791,7 +2801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -2808,7 +2818,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>92</v>
       </c>
@@ -2825,7 +2835,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -2842,7 +2852,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -2859,7 +2869,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>98</v>
       </c>
@@ -2876,7 +2886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -2893,7 +2903,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>102</v>
       </c>
@@ -2910,7 +2920,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -2927,7 +2937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -2944,7 +2954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -2961,7 +2971,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -2978,7 +2988,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -2995,7 +3005,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>114</v>
       </c>
@@ -3012,7 +3022,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>116</v>
       </c>
@@ -3029,7 +3039,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -3046,7 +3056,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -3063,7 +3073,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>122</v>
       </c>
@@ -3080,7 +3090,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>124</v>
       </c>
@@ -3097,7 +3107,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>33</v>
       </c>
@@ -3114,7 +3124,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>127</v>
       </c>
@@ -3131,7 +3141,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>129</v>
       </c>
@@ -3148,7 +3158,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>131</v>
       </c>
@@ -3165,7 +3175,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>133</v>
       </c>
@@ -3182,7 +3192,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>135</v>
       </c>
@@ -3199,7 +3209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>137</v>
       </c>
@@ -3216,7 +3226,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>139</v>
       </c>
@@ -3233,7 +3243,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>141</v>
       </c>
@@ -3250,7 +3260,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>143</v>
       </c>
@@ -3267,7 +3277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>145</v>
       </c>
@@ -3284,7 +3294,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>147</v>
       </c>
@@ -3301,7 +3311,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>149</v>
       </c>
@@ -3318,7 +3328,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>151</v>
       </c>
@@ -3335,7 +3345,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>153</v>
       </c>
@@ -3352,7 +3362,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>33</v>
       </c>
@@ -3369,7 +3379,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>33</v>
       </c>
@@ -3386,7 +3396,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>158</v>
       </c>
@@ -3403,7 +3413,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>160</v>
       </c>
@@ -3420,7 +3430,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>33</v>
       </c>
@@ -3437,7 +3447,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>163</v>
       </c>
@@ -3454,7 +3464,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>165</v>
       </c>
@@ -3471,7 +3481,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>167</v>
       </c>
@@ -3488,7 +3498,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>33</v>
       </c>
@@ -3505,7 +3515,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>170</v>
       </c>
@@ -3522,7 +3532,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>172</v>
       </c>
@@ -3539,7 +3549,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>174</v>
       </c>
@@ -3556,7 +3566,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>176</v>
       </c>
@@ -3573,7 +3583,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>178</v>
       </c>
@@ -3590,7 +3600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>180</v>
       </c>
@@ -3607,7 +3617,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>33</v>
       </c>
@@ -3624,7 +3634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>183</v>
       </c>
@@ -3641,7 +3651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>185</v>
       </c>
@@ -3658,7 +3668,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>187</v>
       </c>
@@ -3675,7 +3685,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>189</v>
       </c>
@@ -3692,7 +3702,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>191</v>
       </c>
@@ -3709,7 +3719,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>33</v>
       </c>
@@ -3726,7 +3736,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>194</v>
       </c>
@@ -3743,7 +3753,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>33</v>
       </c>
@@ -3760,7 +3770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>197</v>
       </c>
@@ -3777,7 +3787,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>200</v>
       </c>
@@ -3794,7 +3804,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>202</v>
       </c>
@@ -3811,7 +3821,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>204</v>
       </c>
@@ -3828,7 +3838,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>33</v>
       </c>
@@ -3845,7 +3855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>207</v>
       </c>
@@ -3862,7 +3872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>33</v>
       </c>
@@ -3879,7 +3889,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>210</v>
       </c>
@@ -3896,7 +3906,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>212</v>
       </c>
@@ -3913,7 +3923,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>214</v>
       </c>
@@ -3930,7 +3940,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>33</v>
       </c>
@@ -3947,7 +3957,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -3964,7 +3974,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>218</v>
       </c>
@@ -3981,7 +3991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>220</v>
       </c>
@@ -3998,7 +4008,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>222</v>
       </c>
@@ -4015,7 +4025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>33</v>
       </c>
@@ -4032,7 +4042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>225</v>
       </c>
@@ -4049,7 +4059,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>227</v>
       </c>
@@ -4066,7 +4076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>229</v>
       </c>
@@ -4083,7 +4093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>231</v>
       </c>
@@ -4100,7 +4110,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -4117,7 +4127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>33</v>
       </c>
@@ -4134,7 +4144,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>33</v>
       </c>
@@ -4151,7 +4161,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>237</v>
       </c>
@@ -4168,7 +4178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>239</v>
       </c>
@@ -4185,7 +4195,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>241</v>
       </c>
@@ -4202,7 +4212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>376</v>
       </c>
@@ -4219,7 +4229,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>244</v>
       </c>
@@ -4236,7 +4246,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>33</v>
       </c>
@@ -4253,7 +4263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>33</v>
       </c>
@@ -4270,7 +4280,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>248</v>
       </c>
@@ -4287,7 +4297,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>250</v>
       </c>
@@ -4304,7 +4314,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>252</v>
       </c>
@@ -4321,7 +4331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>254</v>
       </c>
@@ -4338,7 +4348,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>256</v>
       </c>
@@ -4355,7 +4365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>258</v>
       </c>
@@ -4372,7 +4382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>260</v>
       </c>
@@ -4389,7 +4399,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>262</v>
       </c>
@@ -4406,7 +4416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>33</v>
       </c>
@@ -4423,7 +4433,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>265</v>
       </c>
@@ -4440,7 +4450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>233</v>
       </c>
@@ -4457,7 +4467,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>268</v>
       </c>
@@ -4474,7 +4484,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>270</v>
       </c>
@@ -4491,7 +4501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>272</v>
       </c>
@@ -4508,7 +4518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>274</v>
       </c>
@@ -4525,7 +4535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>276</v>
       </c>
@@ -4542,7 +4552,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>278</v>
       </c>
@@ -4559,7 +4569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>33</v>
       </c>
@@ -4576,7 +4586,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>281</v>
       </c>
@@ -4593,7 +4603,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>33</v>
       </c>
@@ -4610,7 +4620,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>285</v>
       </c>
@@ -4627,7 +4637,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>285</v>
       </c>
@@ -4644,7 +4654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>288</v>
       </c>
@@ -4661,7 +4671,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>33</v>
       </c>
@@ -4678,7 +4688,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>291</v>
       </c>
@@ -4695,7 +4705,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>293</v>
       </c>
@@ -4712,7 +4722,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>295</v>
       </c>
@@ -4729,7 +4739,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>297</v>
       </c>
@@ -4746,7 +4756,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>299</v>
       </c>
@@ -4763,7 +4773,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>301</v>
       </c>
@@ -4780,7 +4790,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>303</v>
       </c>
@@ -4797,7 +4807,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>33</v>
       </c>
@@ -4814,7 +4824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>33</v>
       </c>
@@ -4831,7 +4841,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>307</v>
       </c>
@@ -4848,7 +4858,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>33</v>
       </c>
@@ -4865,7 +4875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>310</v>
       </c>
@@ -4882,7 +4892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>33</v>
       </c>
@@ -4899,7 +4909,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>313</v>
       </c>
@@ -4915,8 +4925,11 @@
       <c r="E173" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F173" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>33</v>
       </c>
@@ -4933,7 +4946,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>316</v>
       </c>
@@ -4949,8 +4962,11 @@
       <c r="E175" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F175" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>318</v>
       </c>
@@ -4966,8 +4982,11 @@
       <c r="E176" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F176" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>319</v>
       </c>
@@ -4984,7 +5003,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>33</v>
       </c>
@@ -5001,7 +5020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>322</v>
       </c>
@@ -5018,7 +5037,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>324</v>
       </c>
@@ -5035,7 +5054,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>33</v>
       </c>
@@ -5052,7 +5071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>327</v>
       </c>
@@ -5069,7 +5088,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>33</v>
       </c>
@@ -5086,7 +5105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>330</v>
       </c>
@@ -5103,7 +5122,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>33</v>
       </c>
@@ -5120,7 +5139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>33</v>
       </c>
@@ -5137,7 +5156,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>334</v>
       </c>
@@ -5154,7 +5173,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>336</v>
       </c>
@@ -5171,7 +5190,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>338</v>
       </c>
@@ -5188,7 +5207,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>340</v>
       </c>
@@ -5205,7 +5224,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>33</v>
       </c>
@@ -5222,7 +5241,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>343</v>
       </c>
@@ -5239,7 +5258,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>33</v>
       </c>
@@ -5256,7 +5275,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>346</v>
       </c>
@@ -5273,7 +5292,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>33</v>
       </c>
@@ -5290,7 +5309,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>349</v>
       </c>
@@ -5307,7 +5326,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>351</v>
       </c>
@@ -5324,7 +5343,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>353</v>
       </c>
@@ -5341,7 +5360,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>355</v>
       </c>
@@ -5358,7 +5377,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>33</v>
       </c>
@@ -5375,7 +5394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>358</v>
       </c>
@@ -5392,7 +5411,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>360</v>
       </c>
@@ -5409,7 +5428,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>362</v>
       </c>
@@ -5426,7 +5445,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>33</v>
       </c>
@@ -5443,7 +5462,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>33</v>
       </c>
@@ -5460,7 +5479,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>366</v>
       </c>
@@ -5477,7 +5496,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>368</v>
       </c>
@@ -5494,7 +5513,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>370</v>
       </c>
@@ -5511,7 +5530,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>372</v>
       </c>
@@ -5528,7 +5547,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>374</v>
       </c>

</xml_diff>

<commit_message>
Column indicating reopening populated using lower case.
</commit_message>
<xml_diff>
--- a/xlsx/feature_timeline.xlsx
+++ b/xlsx/feature_timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kend/Documents/General Maps/Time Line/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\prototype-historical-map\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E494E7C-EF1A-A848-8FC6-D8FE521B334C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C57D62-0101-4226-B051-079BC1FFBB1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="feature_timeline" sheetId="1" r:id="rId1"/>
@@ -1156,7 +1156,7 @@
     <t>reopening</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -1999,20 +1999,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="F176" sqref="F176"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="F177" sqref="F177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>57</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>59</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2597,7 +2597,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>73</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>82</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>84</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>90</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>92</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>98</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>100</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>102</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>110</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>112</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>114</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>116</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>120</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>122</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>124</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>33</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>127</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>129</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>131</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>133</v>
       </c>
@@ -3192,7 +3192,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>135</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>137</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>139</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>141</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>143</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>145</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>147</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>149</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>151</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>153</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>33</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>33</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>158</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>160</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>33</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>163</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>165</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>167</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>33</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>170</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>172</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>174</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>176</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>178</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>180</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>33</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>183</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>185</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>187</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>189</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>191</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>33</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>194</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>33</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>197</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>200</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>202</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>204</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>33</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>207</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>33</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>210</v>
       </c>
@@ -3906,7 +3906,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>212</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>214</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>33</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -3974,7 +3974,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>218</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>220</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>222</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>33</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>225</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>227</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>229</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>231</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>233</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>33</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>33</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>237</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>239</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>241</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>376</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>244</v>
       </c>
@@ -4246,7 +4246,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>33</v>
       </c>
@@ -4263,7 +4263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>33</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>248</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>250</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>252</v>
       </c>
@@ -4331,7 +4331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>254</v>
       </c>
@@ -4348,7 +4348,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>256</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>258</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>260</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>262</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>33</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>265</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>233</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>268</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>270</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>272</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>274</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>276</v>
       </c>
@@ -4552,7 +4552,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>278</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>33</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>281</v>
       </c>
@@ -4603,7 +4603,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>33</v>
       </c>
@@ -4620,7 +4620,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>285</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>285</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>288</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>33</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>291</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>293</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>295</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>297</v>
       </c>
@@ -4756,7 +4756,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>299</v>
       </c>
@@ -4773,7 +4773,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>301</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>303</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>33</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>33</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>307</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>33</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>310</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>33</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>313</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>33</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>316</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>318</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>319</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>33</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>322</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>324</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>33</v>
       </c>
@@ -5071,7 +5071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>327</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>33</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>330</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>33</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>33</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>334</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>336</v>
       </c>
@@ -5190,7 +5190,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>338</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>340</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>33</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>343</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>33</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>346</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>33</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>349</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>351</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>353</v>
       </c>
@@ -5360,7 +5360,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>355</v>
       </c>
@@ -5377,7 +5377,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>33</v>
       </c>
@@ -5394,7 +5394,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>358</v>
       </c>
@@ -5411,7 +5411,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>360</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>362</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>33</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>33</v>
       </c>
@@ -5479,7 +5479,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>366</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>368</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>370</v>
       </c>
@@ -5530,7 +5530,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>372</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>374</v>
       </c>

</xml_diff>